<commit_message>
Added generator of test instances.
Missing parametrization for the amount of constrictions to be generated.

Fixed bug where the resulting files did not have one header.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9912D8E-011F-43DE-9FB0-402251857249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1AB966-8CCF-4EB4-82CE-39AEF8799AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="400">
   <si>
     <t>ID</t>
   </si>
@@ -1308,6 +1308,9 @@
   <si>
     <t>Cumplida?</t>
   </si>
+  <si>
+    <t>Cumplida</t>
+  </si>
 </sst>
 </file>
 
@@ -1317,7 +1320,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1386,6 +1389,14 @@
       <strike/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1883,7 +1894,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2026,6 +2037,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2491,7 +2503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
@@ -6849,8 +6861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
   <dimension ref="B2:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:D36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6966,7 +6978,7 @@
         <v>384</v>
       </c>
       <c r="D13" s="107" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -6996,26 +7008,29 @@
       </c>
       <c r="D16" s="100"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="94"/>
       <c r="C17" s="103"/>
       <c r="D17" s="85"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="120"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="111" t="s">
         <v>382</v>
       </c>
       <c r="C20" s="111"/>
       <c r="D20" s="111"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="111" t="s">
         <v>389</v>
       </c>
       <c r="C21" s="111"/>
       <c r="D21" s="111"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
         <v>386</v>
       </c>
@@ -7026,7 +7041,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="97">
         <v>1</v>
       </c>
@@ -7035,7 +7050,7 @@
       </c>
       <c r="D23" s="97"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="98">
         <v>2</v>
       </c>
@@ -7044,30 +7059,30 @@
       </c>
       <c r="D24" s="98"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="105"/>
       <c r="C25" s="96"/>
       <c r="D25" s="106"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="30"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="111" t="s">
         <v>395</v>
       </c>
       <c r="C28" s="111"/>
       <c r="D28" s="111"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="111" t="s">
         <v>390</v>
       </c>
       <c r="C29" s="111"/>
       <c r="D29" s="111"/>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
         <v>383</v>
       </c>
@@ -7078,7 +7093,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="97">
         <v>23</v>
       </c>
@@ -7087,7 +7102,7 @@
       </c>
       <c r="D31" s="40"/>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="103"/>
       <c r="C32" s="85"/>
       <c r="D32" s="85"/>

</xml_diff>

<commit_message>
Added new type of UserConstriction. Day Interval.
The new type of Constriction allows the user to specify a date interval in which an exam must take place.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1AB966-8CCF-4EB4-82CE-39AEF8799AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41AAD9D-33CA-4582-8B80-899AC1F58B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="405">
   <si>
     <t>ID</t>
   </si>
@@ -1310,6 +1310,21 @@
   </si>
   <si>
     <t>Cumplida</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>Interval initial date</t>
+  </si>
+  <si>
+    <t>Interval ending date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>El examen debe ser fechado en el intervalo de fechas dado</t>
   </si>
 </sst>
 </file>
@@ -1894,7 +1909,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2007,6 +2022,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2037,62 +2053,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2156,6 +2137,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2182,23 +2214,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="21"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2607,10 +2639,10 @@
       <c r="Q5" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="110" t="s">
+      <c r="R5" s="111" t="s">
         <v>299</v>
       </c>
-      <c r="S5" s="110"/>
+      <c r="S5" s="111"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -6822,32 +6854,32 @@
     <mergeCell ref="R5:S5"/>
   </mergeCells>
   <conditionalFormatting sqref="R10 R8:S9 R11:S33 R34 R35:S67 A7:N43 A6:J6 L6:S6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:Q67 Q7:S7 O7:P67">
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>$T6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R6:R67">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$R6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$R44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="19" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$R58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6859,10 +6891,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="B2:E42"/>
+  <dimension ref="B2:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6873,20 +6905,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="111" t="s">
+      <c r="B2" s="112" t="s">
         <v>380</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="112" t="s">
         <v>388</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="101" t="s">
@@ -6957,18 +6989,18 @@
       <c r="E9" s="85"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="118" t="s">
         <v>381</v>
       </c>
-      <c r="C11" s="118"/>
-      <c r="D11" s="119"/>
+      <c r="C11" s="119"/>
+      <c r="D11" s="120"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="114" t="s">
+      <c r="B12" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="C12" s="115"/>
-      <c r="D12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="117"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -7014,21 +7046,21 @@
       <c r="D17" s="85"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="120"/>
+      <c r="E19" s="110"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="111" t="s">
+      <c r="B20" s="112" t="s">
         <v>382</v>
       </c>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="111" t="s">
+      <c r="B21" s="112" t="s">
         <v>389</v>
       </c>
-      <c r="C21" s="111"/>
-      <c r="D21" s="111"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
@@ -7069,18 +7101,18 @@
       <c r="D26" s="5"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="111" t="s">
+      <c r="B28" s="112" t="s">
         <v>395</v>
       </c>
-      <c r="C28" s="111"/>
-      <c r="D28" s="111"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="112"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="111" t="s">
+      <c r="B29" s="112" t="s">
         <v>390</v>
       </c>
-      <c r="C29" s="111"/>
-      <c r="D29" s="111"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="112"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
@@ -7116,18 +7148,18 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="113" t="s">
+      <c r="B35" s="114" t="s">
         <v>391</v>
       </c>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
+      <c r="C35" s="114"/>
+      <c r="D35" s="114"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="112" t="s">
+      <c r="B36" s="113" t="s">
         <v>392</v>
       </c>
-      <c r="C36" s="112"/>
-      <c r="D36" s="112"/>
+      <c r="C36" s="113"/>
+      <c r="D36" s="113"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="101" t="s">
@@ -7159,14 +7191,53 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="B41" s="121" t="s">
+        <v>400</v>
+      </c>
+      <c r="C41" s="121"/>
+      <c r="D41" s="121"/>
+      <c r="E41" s="121"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D42" s="5"/>
+      <c r="B42" s="121" t="s">
+        <v>404</v>
+      </c>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
+      <c r="E42" s="121"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>386</v>
+      </c>
+      <c r="C43" t="s">
+        <v>401</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E43" s="36" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>53</v>
+      </c>
+      <c r="C44" s="14">
+        <v>44363</v>
+      </c>
+      <c r="D44" s="14">
+        <v>44364</v>
+      </c>
+      <c r="E44" t="s">
+        <v>403</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B41:E41"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B35:D35"/>
@@ -7178,6 +7249,16 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B3:E3"/>
   </mergeCells>
+  <conditionalFormatting sqref="C44">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$Q44=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$Q44=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7188,7 +7269,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7283,7 +7364,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7479,7 +7560,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Round input redefined and now configured on the excel.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41AAD9D-33CA-4582-8B80-899AC1F58B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE2D22F-C7B0-4887-9617-1F39F3645847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="26430" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="ListaExámenes2020-2021paraCSV" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">planificación!$A$5:$S$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">planificación!$A$5:$T$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="407">
   <si>
     <t>ID</t>
   </si>
@@ -927,9 +927,6 @@
   </si>
   <si>
     <t>ED</t>
-  </si>
-  <si>
-    <t>SI</t>
   </si>
   <si>
     <t>SDI</t>
@@ -1325,6 +1322,15 @@
   </si>
   <si>
     <t>El examen debe ser fechado en el intervalo de fechas dado</t>
+  </si>
+  <si>
+    <t>Tanda</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -1909,7 +1915,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2026,6 +2032,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2053,9 +2062,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2533,10 +2540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y67"/>
+  <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="P63" sqref="P63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,38 +2563,39 @@
     <col min="13" max="13" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7.28515625" customWidth="1"/>
     <col min="15" max="15" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.28515625" style="3" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.42578125" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" customWidth="1"/>
-    <col min="21" max="23" width="11.42578125" customWidth="1"/>
+    <col min="16" max="18" width="7.28515625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" customWidth="1"/>
+    <col min="22" max="24" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
-        <v>370</v>
-      </c>
-      <c r="S1" s="53"/>
-    </row>
-    <row r="2" spans="1:25" ht="21" x14ac:dyDescent="0.35">
+        <v>369</v>
+      </c>
+      <c r="T1" s="53"/>
+    </row>
+    <row r="2" spans="1:26" ht="21" x14ac:dyDescent="0.35">
       <c r="E2" s="53" t="s">
+        <v>365</v>
+      </c>
+      <c r="T2" s="53" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
         <v>366</v>
       </c>
-      <c r="S2" s="53" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>367</v>
-      </c>
       <c r="H3" s="54"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="P4"/>
       <c r="Q4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="74" t="s">
         <v>137</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>139</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E5" s="73" t="s">
         <v>5</v>
@@ -2622,16 +2630,16 @@
         <v>258</v>
       </c>
       <c r="L5" s="74" t="s">
+        <v>353</v>
+      </c>
+      <c r="M5" s="73" t="s">
         <v>354</v>
       </c>
-      <c r="M5" s="73" t="s">
+      <c r="N5" s="73" t="s">
         <v>355</v>
       </c>
-      <c r="N5" s="73" t="s">
-        <v>356</v>
-      </c>
       <c r="O5" s="73" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="P5" s="92" t="s">
         <v>281</v>
@@ -2639,12 +2647,15 @@
       <c r="Q5" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="111" t="s">
-        <v>299</v>
-      </c>
-      <c r="S5" s="111"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R5" s="92" t="s">
+        <v>404</v>
+      </c>
+      <c r="S5" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="T5" s="111"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
         <v>3</v>
       </c>
@@ -2652,7 +2663,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D6" s="76" t="s">
         <v>267</v>
@@ -2664,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="76" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H6" s="76" t="s">
         <v>136</v>
@@ -2694,21 +2705,24 @@
       <c r="Q6" s="77">
         <v>0</v>
       </c>
-      <c r="R6" s="76" t="s">
+      <c r="R6" s="77" t="s">
+        <v>405</v>
+      </c>
+      <c r="S6" s="76" t="s">
         <v>253</v>
       </c>
-      <c r="S6" s="80"/>
-      <c r="T6" s="81" t="e">
+      <c r="T6" s="80"/>
+      <c r="U6" s="81" t="e">
         <f>VLOOKUP(K6,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U6" s="81"/>
       <c r="V6" s="81"/>
       <c r="W6" s="81"/>
       <c r="X6" s="81"/>
-      <c r="Y6" s="82"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y6" s="81"/>
+      <c r="Z6" s="82"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="83">
         <v>2</v>
       </c>
@@ -2722,7 +2736,7 @@
         <v>276</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F7" s="12">
         <v>1</v>
@@ -2760,25 +2774,28 @@
       <c r="Q7" s="13">
         <v>1</v>
       </c>
-      <c r="R7" s="12" t="s">
+      <c r="R7" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="S7" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S7" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="T7" s="5" t="e">
+      <c r="T7" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="U7" s="5" t="e">
         <f>VLOOKUP(K7,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U7" s="5"/>
       <c r="V7" s="5"/>
       <c r="W7" s="5"/>
-      <c r="X7" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y7" s="40"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z7" s="40"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="83">
         <v>3</v>
       </c>
@@ -2830,23 +2847,24 @@
       <c r="Q8" s="77">
         <v>2</v>
       </c>
-      <c r="R8" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S8" s="16"/>
-      <c r="T8" s="5" t="e">
+      <c r="R8" s="8"/>
+      <c r="S8" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T8" s="16"/>
+      <c r="U8" s="5" t="e">
         <f>VLOOKUP(K8,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U8" s="5"/>
       <c r="V8" s="5"/>
       <c r="W8" s="5"/>
-      <c r="X8" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y8" s="40"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z8" s="40"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="83">
         <v>0</v>
       </c>
@@ -2857,7 +2875,7 @@
         <v>144</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>175</v>
@@ -2866,7 +2884,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>136</v>
@@ -2896,21 +2914,24 @@
       <c r="Q9" s="13">
         <v>3</v>
       </c>
-      <c r="R9" s="12" t="s">
+      <c r="R9" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="S9" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S9" s="16"/>
-      <c r="T9" s="5" t="e">
+      <c r="T9" s="16"/>
+      <c r="U9" s="5" t="e">
         <f>VLOOKUP(K9,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U9" s="5"/>
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
       <c r="X9" s="5"/>
-      <c r="Y9" s="40"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y9" s="5"/>
+      <c r="Z9" s="40"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="83">
         <v>2</v>
       </c>
@@ -2918,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D10" s="12" t="s">
         <v>264</v>
@@ -2962,29 +2983,30 @@
       <c r="Q10" s="77">
         <v>4</v>
       </c>
-      <c r="R10" s="58" t="s">
+      <c r="R10" s="8"/>
+      <c r="S10" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="S10" s="59" t="s">
-        <v>297</v>
-      </c>
-      <c r="T10" s="5" t="e">
+      <c r="T10" s="59" t="s">
+        <v>296</v>
+      </c>
+      <c r="U10" s="5" t="e">
         <f>VLOOKUP(K10,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="W10" s="5">
+      <c r="V10" s="5"/>
+      <c r="W10" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="X10" s="5">
         <v>60</v>
       </c>
-      <c r="X10" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y10" s="40"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y10" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z10" s="40"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="83">
         <v>3</v>
       </c>
@@ -2995,16 +3017,14 @@
         <v>168</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="F11" s="12">
-        <v>1</v>
-      </c>
+      <c r="F11" s="12"/>
       <c r="G11" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>136</v>
@@ -3034,21 +3054,24 @@
       <c r="Q11" s="13">
         <v>5</v>
       </c>
-      <c r="R11" s="12" t="s">
+      <c r="R11" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="S11" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S11" s="19"/>
-      <c r="T11" s="5" t="e">
+      <c r="T11" s="19"/>
+      <c r="U11" s="5" t="e">
         <f>VLOOKUP(K11,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U11" s="5"/>
       <c r="V11" s="5"/>
       <c r="W11" s="5"/>
       <c r="X11" s="5"/>
-      <c r="Y11" s="40"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y11" s="5"/>
+      <c r="Z11" s="40"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="83">
         <v>4</v>
       </c>
@@ -3058,9 +3081,7 @@
       <c r="C12" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>283</v>
-      </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
         <v>198</v>
       </c>
@@ -3100,23 +3121,24 @@
       <c r="Q12" s="77">
         <v>6</v>
       </c>
-      <c r="R12" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S12" s="16"/>
-      <c r="T12" s="5" t="e">
+      <c r="R12" s="8"/>
+      <c r="S12" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T12" s="16"/>
+      <c r="U12" s="5" t="e">
         <f>VLOOKUP(K12,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U12" s="5"/>
       <c r="V12" s="5"/>
       <c r="W12" s="5"/>
-      <c r="X12" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y12" s="40"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z12" s="40"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="83">
         <v>2</v>
       </c>
@@ -3168,27 +3190,30 @@
       <c r="Q13" s="13">
         <v>7</v>
       </c>
-      <c r="R13" s="12" t="s">
+      <c r="R13" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="S13" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S13" s="16" t="s">
-        <v>339</v>
-      </c>
-      <c r="T13" s="5" t="e">
+      <c r="T13" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="U13" s="5" t="e">
         <f>VLOOKUP(K13,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U13" s="5"/>
       <c r="V13" s="5"/>
       <c r="W13" s="5"/>
-      <c r="X13" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y13" s="40" t="s">
+      <c r="X13" s="5"/>
+      <c r="Y13" s="36" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z13" s="40" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="83">
         <v>1</v>
       </c>
@@ -3207,9 +3232,7 @@
       <c r="F14" s="12">
         <v>1</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="G14" s="12"/>
       <c r="H14" s="12" t="s">
         <v>22</v>
       </c>
@@ -3240,34 +3263,35 @@
       <c r="Q14" s="77">
         <v>8</v>
       </c>
-      <c r="R14" s="12" t="s">
+      <c r="R14" s="8" t="s">
+        <v>406</v>
+      </c>
+      <c r="S14" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S14" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="T14" s="5" t="e">
+      <c r="T14" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="U14" s="5" t="e">
         <f>VLOOKUP(K14,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U14" s="5"/>
       <c r="V14" s="5"/>
       <c r="W14" s="5"/>
-      <c r="X14" s="88" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y14" s="40"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X14" s="5"/>
+      <c r="Y14" s="88" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z14" s="40"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="83">
         <v>3</v>
       </c>
       <c r="B15" s="12">
         <v>1</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>302</v>
-      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="12" t="s">
         <v>267</v>
       </c>
@@ -3308,21 +3332,22 @@
       <c r="Q15" s="13">
         <v>9</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="R15" s="13"/>
+      <c r="S15" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S15" s="16"/>
-      <c r="T15" s="5" t="e">
+      <c r="T15" s="16"/>
+      <c r="U15" s="5" t="e">
         <f>VLOOKUP(K15,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U15" s="5"/>
       <c r="V15" s="5"/>
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
-      <c r="Y15" s="40"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y15" s="5"/>
+      <c r="Z15" s="40"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="83">
         <v>4</v>
       </c>
@@ -3374,25 +3399,26 @@
       <c r="Q16" s="77">
         <v>10</v>
       </c>
-      <c r="R16" s="12" t="s">
+      <c r="R16" s="8"/>
+      <c r="S16" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S16" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="T16" s="5" t="e">
+      <c r="T16" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="U16" s="5" t="e">
         <f>VLOOKUP(K16,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U16" s="5"/>
       <c r="V16" s="5"/>
       <c r="W16" s="5"/>
-      <c r="X16" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y16" s="40"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X16" s="5"/>
+      <c r="Y16" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z16" s="40"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="83">
         <v>3</v>
       </c>
@@ -3444,25 +3470,26 @@
       <c r="Q17" s="13">
         <v>11</v>
       </c>
-      <c r="R17" s="12" t="s">
+      <c r="R17" s="13"/>
+      <c r="S17" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S17" s="46" t="s">
-        <v>348</v>
-      </c>
-      <c r="T17" s="5" t="e">
+      <c r="T17" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="U17" s="5" t="e">
         <f>VLOOKUP(K17,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U17" s="5"/>
       <c r="V17" s="5"/>
       <c r="W17" s="5"/>
-      <c r="X17" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y17" s="40"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X17" s="5"/>
+      <c r="Y17" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z17" s="40"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="83">
         <v>2</v>
       </c>
@@ -3470,7 +3497,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D18" s="12" t="s">
         <v>282</v>
@@ -3514,27 +3541,28 @@
       <c r="Q18" s="77">
         <v>12</v>
       </c>
-      <c r="R18" s="12" t="s">
+      <c r="R18" s="8"/>
+      <c r="S18" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S18" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="T18" s="5" t="e">
+      <c r="T18" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="U18" s="5" t="e">
         <f>VLOOKUP(K18,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U18" s="5"/>
       <c r="V18" s="5"/>
       <c r="W18" s="5"/>
-      <c r="X18" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y18" s="40" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X18" s="5"/>
+      <c r="Y18" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z18" s="40" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="83">
         <v>0</v>
       </c>
@@ -3545,7 +3573,7 @@
         <v>204</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>175</v>
@@ -3554,7 +3582,7 @@
         <v>2</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>136</v>
@@ -3584,21 +3612,22 @@
       <c r="Q19" s="13">
         <v>13</v>
       </c>
-      <c r="R19" s="12" t="s">
+      <c r="R19" s="13"/>
+      <c r="S19" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S19" s="43"/>
-      <c r="T19" s="5" t="e">
+      <c r="T19" s="43"/>
+      <c r="U19" s="5" t="e">
         <f>VLOOKUP(K19,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U19" s="5"/>
       <c r="V19" s="5"/>
       <c r="W19" s="5"/>
       <c r="X19" s="5"/>
-      <c r="Y19" s="40"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y19" s="5"/>
+      <c r="Z19" s="40"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="83">
         <v>1</v>
       </c>
@@ -3648,25 +3677,26 @@
       <c r="Q20" s="77">
         <v>14</v>
       </c>
-      <c r="R20" s="12" t="s">
+      <c r="R20" s="8"/>
+      <c r="S20" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S20" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="T20" s="5" t="e">
+      <c r="T20" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="U20" s="5" t="e">
         <f>VLOOKUP(K20,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U20" s="5"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="88" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y20" s="40"/>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X20" s="5"/>
+      <c r="Y20" s="88" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z20" s="40"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="83">
         <v>3</v>
       </c>
@@ -3677,7 +3707,7 @@
         <v>153</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E21" s="62" t="s">
         <v>184</v>
@@ -3718,25 +3748,26 @@
       <c r="Q21" s="13">
         <v>15</v>
       </c>
-      <c r="R21" s="12" t="s">
+      <c r="R21" s="13"/>
+      <c r="S21" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S21" s="19" t="s">
-        <v>337</v>
-      </c>
-      <c r="T21" s="5" t="e">
+      <c r="T21" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="U21" s="5" t="e">
         <f>VLOOKUP(K21,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U21" s="5"/>
       <c r="V21" s="5"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y21" s="40"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X21" s="5"/>
+      <c r="Y21" s="36" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z21" s="40"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="84">
         <v>2</v>
       </c>
@@ -3788,21 +3819,22 @@
       <c r="Q22" s="77">
         <v>16</v>
       </c>
-      <c r="R22" s="65" t="s">
+      <c r="R22" s="122"/>
+      <c r="S22" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="S22" s="70"/>
-      <c r="T22" s="71" t="e">
+      <c r="T22" s="70"/>
+      <c r="U22" s="71" t="e">
         <f>VLOOKUP(K22,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U22" s="71"/>
       <c r="V22" s="71"/>
       <c r="W22" s="71"/>
       <c r="X22" s="71"/>
-      <c r="Y22" s="85"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y22" s="71"/>
+      <c r="Z22" s="85"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="75">
         <v>1</v>
       </c>
@@ -3854,25 +3886,26 @@
       <c r="Q23" s="13">
         <v>17</v>
       </c>
-      <c r="R23" s="76" t="s">
+      <c r="R23" s="8"/>
+      <c r="S23" s="76" t="s">
         <v>255</v>
       </c>
-      <c r="S23" s="86" t="s">
-        <v>338</v>
-      </c>
-      <c r="T23" s="81" t="e">
+      <c r="T23" s="86" t="s">
+        <v>337</v>
+      </c>
+      <c r="U23" s="81" t="e">
         <f>VLOOKUP(K23,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U23" s="81"/>
       <c r="V23" s="81"/>
       <c r="W23" s="81"/>
-      <c r="X23" s="90" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y23" s="82"/>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X23" s="81"/>
+      <c r="Y23" s="90" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z23" s="82"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="83">
         <v>2</v>
       </c>
@@ -3924,25 +3957,26 @@
       <c r="Q24" s="77">
         <v>18</v>
       </c>
-      <c r="R24" s="12" t="s">
+      <c r="R24" s="8"/>
+      <c r="S24" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S24" s="19" t="s">
+      <c r="T24" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="T24" s="5" t="e">
+      <c r="U24" s="5" t="e">
         <f>VLOOKUP(K24,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U24" s="5"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y24" s="40"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z24" s="40"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="83">
         <v>0</v>
       </c>
@@ -3953,7 +3987,7 @@
         <v>208</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>189</v>
@@ -3992,21 +4026,22 @@
       <c r="Q25" s="13">
         <v>19</v>
       </c>
-      <c r="R25" s="12" t="s">
+      <c r="R25" s="13"/>
+      <c r="S25" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S25" s="16"/>
-      <c r="T25" s="5" t="e">
+      <c r="T25" s="16"/>
+      <c r="U25" s="5" t="e">
         <f>VLOOKUP(K25,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U25" s="5"/>
       <c r="V25" s="5"/>
       <c r="W25" s="5"/>
       <c r="X25" s="5"/>
-      <c r="Y25" s="40"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="40"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="83">
         <v>0</v>
       </c>
@@ -4017,7 +4052,7 @@
         <v>208</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>189</v>
@@ -4026,7 +4061,7 @@
         <v>2</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>136</v>
@@ -4056,23 +4091,24 @@
       <c r="Q26" s="77">
         <v>20</v>
       </c>
-      <c r="R26" s="12" t="s">
+      <c r="R26" s="8"/>
+      <c r="S26" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S26" s="19"/>
-      <c r="T26" s="5" t="e">
+      <c r="T26" s="19"/>
+      <c r="U26" s="5" t="e">
         <f>VLOOKUP(K26,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U26" s="5" t="s">
-        <v>318</v>
-      </c>
-      <c r="V26" s="5"/>
+      <c r="V26" s="5" t="s">
+        <v>317</v>
+      </c>
       <c r="W26" s="5"/>
       <c r="X26" s="5"/>
-      <c r="Y26" s="40"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="40"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="83">
         <v>3</v>
       </c>
@@ -4122,21 +4158,22 @@
       <c r="Q27" s="13">
         <v>21</v>
       </c>
-      <c r="R27" s="12" t="s">
+      <c r="R27" s="13"/>
+      <c r="S27" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S27" s="16"/>
-      <c r="T27" s="5" t="e">
+      <c r="T27" s="16"/>
+      <c r="U27" s="5" t="e">
         <f>VLOOKUP(K27,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
       <c r="X27" s="5"/>
-      <c r="Y27" s="40"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="40"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="83">
         <v>3</v>
       </c>
@@ -4156,10 +4193,10 @@
         <v>2</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="15">
@@ -4186,21 +4223,22 @@
       <c r="Q28" s="77">
         <v>22</v>
       </c>
-      <c r="R28" s="12" t="s">
+      <c r="R28" s="8"/>
+      <c r="S28" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S28" s="23"/>
-      <c r="T28" s="5" t="e">
+      <c r="T28" s="23"/>
+      <c r="U28" s="5" t="e">
         <f>VLOOKUP(K28,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U28" s="5"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5"/>
-      <c r="Y28" s="40"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="40"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="87">
         <v>1</v>
       </c>
@@ -4208,13 +4246,13 @@
         <v>2</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E29" s="57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F29" s="33">
         <v>1</v>
@@ -4250,29 +4288,30 @@
       <c r="Q29" s="13">
         <v>23</v>
       </c>
-      <c r="R29" s="58" t="s">
+      <c r="R29" s="13"/>
+      <c r="S29" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="S29" s="61" t="s">
-        <v>297</v>
-      </c>
-      <c r="T29" s="5" t="e">
+      <c r="T29" s="61" t="s">
+        <v>296</v>
+      </c>
+      <c r="U29" s="5" t="e">
         <f>VLOOKUP(K29,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="W29" s="5">
+      <c r="V29" s="5"/>
+      <c r="W29" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="X29" s="5">
         <v>60</v>
       </c>
-      <c r="X29" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y29" s="40"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y29" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z29" s="40"/>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="83">
         <v>2</v>
       </c>
@@ -4324,23 +4363,24 @@
       <c r="Q30" s="77">
         <v>24</v>
       </c>
-      <c r="R30" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S30" s="16"/>
-      <c r="T30" s="5" t="e">
+      <c r="R30" s="8"/>
+      <c r="S30" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T30" s="16"/>
+      <c r="U30" s="5" t="e">
         <f>VLOOKUP(K30,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U30" s="5"/>
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
-      <c r="X30" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y30" s="40"/>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z30" s="40"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="83">
         <v>0</v>
       </c>
@@ -4348,13 +4388,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>275</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F31" s="12">
         <v>1</v>
@@ -4392,21 +4432,22 @@
       <c r="Q31" s="13">
         <v>25</v>
       </c>
-      <c r="R31" s="12" t="s">
+      <c r="R31" s="13"/>
+      <c r="S31" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S31" s="16"/>
-      <c r="T31" s="5" t="e">
+      <c r="T31" s="16"/>
+      <c r="U31" s="5" t="e">
         <f>VLOOKUP(K31,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U31" s="5"/>
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
       <c r="X31" s="5"/>
-      <c r="Y31" s="40"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="40"/>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="83">
         <v>1</v>
       </c>
@@ -4458,23 +4499,24 @@
       <c r="Q32" s="77">
         <v>26</v>
       </c>
-      <c r="R32" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S32" s="16"/>
-      <c r="T32" s="5" t="e">
+      <c r="R32" s="8"/>
+      <c r="S32" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T32" s="16"/>
+      <c r="U32" s="5" t="e">
         <f>VLOOKUP(K32,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U32" s="5"/>
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
-      <c r="X32" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y32" s="40"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z32" s="40"/>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="83">
         <v>3</v>
       </c>
@@ -4526,23 +4568,24 @@
       <c r="Q33" s="13">
         <v>27</v>
       </c>
-      <c r="R33" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S33" s="16"/>
-      <c r="T33" s="5" t="e">
+      <c r="R33" s="13"/>
+      <c r="S33" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T33" s="16"/>
+      <c r="U33" s="5" t="e">
         <f>VLOOKUP(K33,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U33" s="5"/>
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
-      <c r="X33" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y33" s="40"/>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z33" s="40"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="83">
         <v>2</v>
       </c>
@@ -4550,7 +4593,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>264</v>
@@ -4594,29 +4637,30 @@
       <c r="Q34" s="77">
         <v>28</v>
       </c>
-      <c r="R34" s="58" t="s">
+      <c r="R34" s="8"/>
+      <c r="S34" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="S34" s="59" t="s">
-        <v>369</v>
-      </c>
-      <c r="T34" s="5" t="e">
+      <c r="T34" s="59" t="s">
+        <v>368</v>
+      </c>
+      <c r="U34" s="5" t="e">
         <f>VLOOKUP(K34,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U34" s="5"/>
-      <c r="V34" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="W34" s="5">
+      <c r="V34" s="5"/>
+      <c r="W34" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="X34" s="5">
         <v>60</v>
       </c>
-      <c r="X34" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y34" s="40"/>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y34" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z34" s="40"/>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="83">
         <v>1</v>
       </c>
@@ -4630,7 +4674,7 @@
         <v>280</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F35" s="12">
         <v>2</v>
@@ -4668,25 +4712,26 @@
       <c r="Q35" s="13">
         <v>29</v>
       </c>
-      <c r="R35" s="12" t="s">
+      <c r="R35" s="13"/>
+      <c r="S35" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S35" s="21" t="s">
-        <v>340</v>
-      </c>
-      <c r="T35" s="5" t="e">
+      <c r="T35" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="U35" s="5" t="e">
         <f>VLOOKUP(K35,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U35" s="5"/>
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
-      <c r="X35" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y35" s="40"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X35" s="5"/>
+      <c r="Y35" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z35" s="40"/>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="83">
         <v>4</v>
       </c>
@@ -4738,25 +4783,26 @@
       <c r="Q36" s="77">
         <v>30</v>
       </c>
-      <c r="R36" s="12" t="s">
+      <c r="R36" s="8"/>
+      <c r="S36" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S36" s="16" t="s">
+      <c r="T36" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="T36" s="5" t="e">
+      <c r="U36" s="5" t="e">
         <f>VLOOKUP(K36,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U36" s="5"/>
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
-      <c r="X36" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y36" s="40"/>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X36" s="5"/>
+      <c r="Y36" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z36" s="40"/>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="83">
         <v>2</v>
       </c>
@@ -4770,7 +4816,7 @@
         <v>276</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F37" s="12">
         <v>1</v>
@@ -4808,25 +4854,26 @@
       <c r="Q37" s="13">
         <v>31</v>
       </c>
-      <c r="R37" s="12" t="s">
+      <c r="R37" s="13"/>
+      <c r="S37" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S37" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="T37" s="5" t="e">
+      <c r="T37" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="U37" s="5" t="e">
         <f>VLOOKUP(K37,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U37" s="5"/>
       <c r="V37" s="5"/>
       <c r="W37" s="5"/>
-      <c r="X37" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y37" s="40"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X37" s="5"/>
+      <c r="Y37" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z37" s="40"/>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="83">
         <v>1</v>
       </c>
@@ -4878,25 +4925,26 @@
       <c r="Q38" s="77">
         <v>32</v>
       </c>
-      <c r="R38" s="12" t="s">
+      <c r="R38" s="8"/>
+      <c r="S38" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S38" s="64" t="s">
-        <v>373</v>
-      </c>
-      <c r="T38" s="5" t="e">
+      <c r="T38" s="64" t="s">
+        <v>372</v>
+      </c>
+      <c r="U38" s="5" t="e">
         <f>VLOOKUP(K38,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U38" s="5"/>
       <c r="V38" s="5"/>
       <c r="W38" s="5"/>
-      <c r="X38" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y38" s="40"/>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X38" s="5"/>
+      <c r="Y38" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z38" s="40"/>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="83">
         <v>3</v>
       </c>
@@ -4946,21 +4994,22 @@
       <c r="Q39" s="13">
         <v>33</v>
       </c>
-      <c r="R39" s="12" t="s">
+      <c r="R39" s="13"/>
+      <c r="S39" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S39" s="16"/>
-      <c r="T39" s="5" t="e">
+      <c r="T39" s="16"/>
+      <c r="U39" s="5" t="e">
         <f>VLOOKUP(K39,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U39" s="5"/>
       <c r="V39" s="5"/>
       <c r="W39" s="5"/>
       <c r="X39" s="5"/>
-      <c r="Y39" s="40"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y39" s="5"/>
+      <c r="Z39" s="40"/>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="83">
         <v>3</v>
       </c>
@@ -4980,7 +5029,7 @@
         <v>2</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>136</v>
@@ -5010,21 +5059,22 @@
       <c r="Q40" s="77">
         <v>34</v>
       </c>
-      <c r="R40" s="12" t="s">
+      <c r="R40" s="8"/>
+      <c r="S40" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S40" s="19"/>
-      <c r="T40" s="5" t="e">
+      <c r="T40" s="19"/>
+      <c r="U40" s="5" t="e">
         <f>VLOOKUP(K40,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U40" s="5"/>
       <c r="V40" s="5"/>
       <c r="W40" s="5"/>
       <c r="X40" s="5"/>
-      <c r="Y40" s="40"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y40" s="5"/>
+      <c r="Z40" s="40"/>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="83">
         <v>2</v>
       </c>
@@ -5032,7 +5082,7 @@
         <v>1</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D41" s="12" t="s">
         <v>282</v>
@@ -5076,25 +5126,26 @@
       <c r="Q41" s="13">
         <v>35</v>
       </c>
-      <c r="R41" s="12" t="s">
+      <c r="R41" s="13"/>
+      <c r="S41" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S41" s="28" t="s">
-        <v>342</v>
-      </c>
-      <c r="T41" s="5" t="e">
+      <c r="T41" s="28" t="s">
+        <v>341</v>
+      </c>
+      <c r="U41" s="5" t="e">
         <f>VLOOKUP(K41,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U41" s="5"/>
       <c r="V41" s="5"/>
       <c r="W41" s="5"/>
-      <c r="X41" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y41" s="40"/>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X41" s="5"/>
+      <c r="Y41" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z41" s="40"/>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="83">
         <v>0</v>
       </c>
@@ -5105,7 +5156,7 @@
         <v>158</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E42" s="12" t="s">
         <v>188</v>
@@ -5114,7 +5165,7 @@
         <v>1</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H42" s="12" t="s">
         <v>136</v>
@@ -5144,21 +5195,22 @@
       <c r="Q42" s="77">
         <v>36</v>
       </c>
-      <c r="R42" s="12" t="s">
+      <c r="R42" s="8"/>
+      <c r="S42" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S42" s="16"/>
-      <c r="T42" s="5" t="e">
+      <c r="T42" s="16"/>
+      <c r="U42" s="5" t="e">
         <f>VLOOKUP(K42,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U42" s="5"/>
       <c r="V42" s="5"/>
       <c r="W42" s="5"/>
       <c r="X42" s="5"/>
-      <c r="Y42" s="40"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y42" s="5"/>
+      <c r="Z42" s="40"/>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="83">
         <v>3</v>
       </c>
@@ -5210,27 +5262,28 @@
       <c r="Q43" s="13">
         <v>37</v>
       </c>
-      <c r="R43" s="12" t="s">
+      <c r="R43" s="13"/>
+      <c r="S43" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S43" s="28" t="s">
-        <v>340</v>
-      </c>
-      <c r="T43" s="5" t="e">
+      <c r="T43" s="28" t="s">
+        <v>339</v>
+      </c>
+      <c r="U43" s="5" t="e">
         <f>VLOOKUP(K43,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U43" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="V43" s="5"/>
+      <c r="V43" s="5" t="s">
+        <v>356</v>
+      </c>
       <c r="W43" s="5"/>
-      <c r="X43" s="89" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y43" s="40"/>
-    </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X43" s="5"/>
+      <c r="Y43" s="89" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z43" s="40"/>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="83">
         <v>1</v>
       </c>
@@ -5241,7 +5294,7 @@
         <v>145</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E44" s="12" t="s">
         <v>176</v>
@@ -5282,25 +5335,26 @@
       <c r="Q44" s="77">
         <v>38</v>
       </c>
-      <c r="R44" s="12" t="s">
+      <c r="R44" s="8"/>
+      <c r="S44" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S44" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="T44" s="5" t="e">
+      <c r="T44" s="16" t="s">
+        <v>336</v>
+      </c>
+      <c r="U44" s="5" t="e">
         <f>VLOOKUP(K44,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U44" s="5"/>
       <c r="V44" s="5"/>
       <c r="W44" s="5"/>
-      <c r="X44" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y44" s="40"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z44" s="40"/>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="83">
         <v>2</v>
       </c>
@@ -5352,25 +5406,26 @@
       <c r="Q45" s="13">
         <v>39</v>
       </c>
-      <c r="R45" s="12" t="s">
+      <c r="R45" s="13"/>
+      <c r="S45" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S45" s="19" t="s">
-        <v>297</v>
-      </c>
-      <c r="T45" s="5" t="e">
+      <c r="T45" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="U45" s="5" t="e">
         <f>VLOOKUP(K45,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U45" s="5"/>
       <c r="V45" s="5"/>
       <c r="W45" s="5"/>
-      <c r="X45" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y45" s="40"/>
-    </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X45" s="5"/>
+      <c r="Y45" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z45" s="40"/>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="83">
         <v>1</v>
       </c>
@@ -5422,23 +5477,24 @@
       <c r="Q46" s="77">
         <v>40</v>
       </c>
-      <c r="R46" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S46" s="19"/>
-      <c r="T46" s="5" t="e">
+      <c r="R46" s="8"/>
+      <c r="S46" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T46" s="19"/>
+      <c r="U46" s="5" t="e">
         <f>VLOOKUP(K46,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U46" s="5"/>
       <c r="V46" s="5"/>
       <c r="W46" s="5"/>
-      <c r="X46" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y46" s="40"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X46" s="5"/>
+      <c r="Y46" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z46" s="40"/>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="83">
         <v>0</v>
       </c>
@@ -5490,21 +5546,22 @@
       <c r="Q47" s="13">
         <v>41</v>
       </c>
-      <c r="R47" s="12" t="s">
+      <c r="R47" s="13"/>
+      <c r="S47" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S47" s="16"/>
-      <c r="T47" s="5" t="e">
+      <c r="T47" s="16"/>
+      <c r="U47" s="5" t="e">
         <f>VLOOKUP(K47,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U47" s="5"/>
       <c r="V47" s="5"/>
       <c r="W47" s="5"/>
       <c r="X47" s="5"/>
-      <c r="Y47" s="40"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="40"/>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="83">
         <v>2</v>
       </c>
@@ -5554,23 +5611,24 @@
       <c r="Q48" s="77">
         <v>42</v>
       </c>
-      <c r="R48" s="12" t="s">
+      <c r="R48" s="8"/>
+      <c r="S48" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S48" s="5"/>
-      <c r="T48" s="5" t="e">
+      <c r="T48" s="5"/>
+      <c r="U48" s="5" t="e">
         <f>VLOOKUP(K48,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U48" s="22" t="s">
-        <v>314</v>
-      </c>
-      <c r="V48" s="5"/>
+      <c r="V48" s="22" t="s">
+        <v>313</v>
+      </c>
       <c r="W48" s="5"/>
       <c r="X48" s="5"/>
-      <c r="Y48" s="40"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="40"/>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="83">
         <v>3</v>
       </c>
@@ -5590,10 +5648,10 @@
         <v>3</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H49" s="12" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="I49" s="13"/>
       <c r="J49" s="15">
@@ -5620,21 +5678,22 @@
       <c r="Q49" s="13">
         <v>43</v>
       </c>
-      <c r="R49" s="12" t="s">
+      <c r="R49" s="13"/>
+      <c r="S49" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S49" s="19"/>
-      <c r="T49" s="5" t="e">
+      <c r="T49" s="19"/>
+      <c r="U49" s="5" t="e">
         <f>VLOOKUP(K49,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U49" s="5"/>
       <c r="V49" s="5"/>
       <c r="W49" s="5"/>
       <c r="X49" s="5"/>
-      <c r="Y49" s="40"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="40"/>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="83">
         <v>1</v>
       </c>
@@ -5686,25 +5745,26 @@
       <c r="Q50" s="77">
         <v>44</v>
       </c>
-      <c r="R50" s="12" t="s">
+      <c r="R50" s="8"/>
+      <c r="S50" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S50" s="29" t="s">
-        <v>343</v>
-      </c>
-      <c r="T50" s="5" t="e">
+      <c r="T50" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="U50" s="5" t="e">
         <f>VLOOKUP(K50,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U50" s="5"/>
       <c r="V50" s="5"/>
       <c r="W50" s="5"/>
-      <c r="X50" s="89" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y50" s="40"/>
-    </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X50" s="5"/>
+      <c r="Y50" s="89" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z50" s="40"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="83">
         <v>4</v>
       </c>
@@ -5712,7 +5772,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D51" s="12" t="s">
         <v>262</v>
@@ -5756,21 +5816,22 @@
       <c r="Q51" s="13">
         <v>45</v>
       </c>
-      <c r="R51" s="12" t="s">
+      <c r="R51" s="13"/>
+      <c r="S51" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S51" s="19"/>
-      <c r="T51" s="5" t="e">
+      <c r="T51" s="19"/>
+      <c r="U51" s="5" t="e">
         <f>VLOOKUP(K51,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U51" s="5"/>
       <c r="V51" s="5"/>
       <c r="W51" s="5"/>
       <c r="X51" s="5"/>
-      <c r="Y51" s="40"/>
-    </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="40"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="83">
         <v>2</v>
       </c>
@@ -5822,25 +5883,26 @@
       <c r="Q52" s="77">
         <v>46</v>
       </c>
-      <c r="R52" s="12" t="s">
+      <c r="R52" s="8"/>
+      <c r="S52" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S52" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="T52" s="5" t="e">
+      <c r="T52" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="U52" s="5" t="e">
         <f>VLOOKUP(K52,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U52" s="5"/>
       <c r="V52" s="5"/>
       <c r="W52" s="5"/>
-      <c r="X52" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y52" s="40"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z52" s="40"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="83">
         <v>1</v>
       </c>
@@ -5892,23 +5954,24 @@
       <c r="Q53" s="13">
         <v>47</v>
       </c>
-      <c r="R53" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="S53" s="16"/>
-      <c r="T53" s="5" t="e">
+      <c r="R53" s="13"/>
+      <c r="S53" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="T53" s="16"/>
+      <c r="U53" s="5" t="e">
         <f>VLOOKUP(K53,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U53" s="5"/>
       <c r="V53" s="5"/>
       <c r="W53" s="5"/>
-      <c r="X53" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="Y53" s="40"/>
-    </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z53" s="40"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="83">
         <v>3</v>
       </c>
@@ -5919,7 +5982,7 @@
         <v>207</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E54" s="62" t="s">
         <v>184</v>
@@ -5958,21 +6021,22 @@
       <c r="Q54" s="77">
         <v>48</v>
       </c>
-      <c r="R54" s="12" t="s">
+      <c r="R54" s="8"/>
+      <c r="S54" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S54" s="23"/>
-      <c r="T54" s="5" t="e">
+      <c r="T54" s="23"/>
+      <c r="U54" s="5" t="e">
         <f>VLOOKUP(K54,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U54" s="5"/>
       <c r="V54" s="5"/>
       <c r="W54" s="5"/>
       <c r="X54" s="5"/>
-      <c r="Y54" s="40"/>
-    </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="40"/>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="83">
         <v>2</v>
       </c>
@@ -6024,25 +6088,26 @@
       <c r="Q55" s="13">
         <v>49</v>
       </c>
-      <c r="R55" s="12" t="s">
+      <c r="R55" s="13"/>
+      <c r="S55" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S55" s="29" t="s">
-        <v>338</v>
-      </c>
-      <c r="T55" s="5" t="e">
+      <c r="T55" s="29" t="s">
+        <v>337</v>
+      </c>
+      <c r="U55" s="5" t="e">
         <f>VLOOKUP(K55,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U55" s="5"/>
       <c r="V55" s="5"/>
       <c r="W55" s="5"/>
-      <c r="X55" s="88" t="s">
-        <v>379</v>
-      </c>
-      <c r="Y55" s="40"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X55" s="5"/>
+      <c r="Y55" s="88" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z55" s="40"/>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="83">
         <v>0</v>
       </c>
@@ -6053,7 +6118,7 @@
         <v>140</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>171</v>
@@ -6062,7 +6127,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>136</v>
@@ -6092,21 +6157,22 @@
       <c r="Q56" s="77">
         <v>50</v>
       </c>
-      <c r="R56" s="12" t="s">
+      <c r="R56" s="8"/>
+      <c r="S56" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="S56" s="16"/>
-      <c r="T56" s="5" t="e">
+      <c r="T56" s="16"/>
+      <c r="U56" s="5" t="e">
         <f>VLOOKUP(K56,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U56" s="5"/>
       <c r="V56" s="5"/>
       <c r="W56" s="5"/>
       <c r="X56" s="5"/>
-      <c r="Y56" s="40"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="40"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="83">
         <v>3</v>
       </c>
@@ -6158,25 +6224,26 @@
       <c r="Q57" s="13">
         <v>51</v>
       </c>
-      <c r="R57" s="12" t="s">
+      <c r="R57" s="13"/>
+      <c r="S57" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S57" s="20" t="s">
-        <v>345</v>
-      </c>
-      <c r="T57" s="5" t="e">
+      <c r="T57" s="20" t="s">
+        <v>344</v>
+      </c>
+      <c r="U57" s="5" t="e">
         <f>VLOOKUP(K57,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U57" s="5"/>
       <c r="V57" s="5"/>
       <c r="W57" s="5"/>
-      <c r="X57" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y57" s="40"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z57" s="40"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="83">
         <v>2</v>
       </c>
@@ -6187,7 +6254,7 @@
         <v>141</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E58" s="12" t="s">
         <v>172</v>
@@ -6228,25 +6295,26 @@
       <c r="Q58" s="77">
         <v>52</v>
       </c>
-      <c r="R58" s="12" t="s">
+      <c r="R58" s="8"/>
+      <c r="S58" s="12" t="s">
         <v>256</v>
       </c>
-      <c r="S58" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="T58" s="5" t="e">
+      <c r="T58" s="16" t="s">
+        <v>296</v>
+      </c>
+      <c r="U58" s="5" t="e">
         <f>VLOOKUP(K58,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U58" s="5"/>
       <c r="V58" s="5"/>
       <c r="W58" s="5"/>
-      <c r="X58" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="Y58" s="40"/>
-    </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z58" s="40"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="84">
         <v>4</v>
       </c>
@@ -6257,10 +6325,10 @@
         <v>165</v>
       </c>
       <c r="D59" s="65" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E59" s="65" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F59" s="65">
         <v>1</v>
@@ -6298,21 +6366,22 @@
       <c r="Q59" s="13">
         <v>53</v>
       </c>
-      <c r="R59" s="65" t="s">
+      <c r="R59" s="26"/>
+      <c r="S59" s="65" t="s">
         <v>253</v>
       </c>
-      <c r="S59" s="70"/>
-      <c r="T59" s="71" t="e">
+      <c r="T59" s="70"/>
+      <c r="U59" s="71" t="e">
         <f>VLOOKUP(K59,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U59" s="71"/>
       <c r="V59" s="71"/>
       <c r="W59" s="71"/>
       <c r="X59" s="71"/>
-      <c r="Y59" s="85"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y59" s="71"/>
+      <c r="Z59" s="85"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="6">
         <v>0</v>
       </c>
@@ -6320,10 +6389,10 @@
         <v>1</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E60" s="7" t="s">
         <v>251</v>
@@ -6332,7 +6401,7 @@
         <v>1</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>136</v>
@@ -6362,16 +6431,17 @@
       <c r="Q60" s="77">
         <v>54</v>
       </c>
-      <c r="R60" s="7" t="s">
+      <c r="R60" s="8"/>
+      <c r="S60" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="S60" s="72"/>
-      <c r="T60" t="e">
+      <c r="T60" s="72"/>
+      <c r="U60" t="e">
         <f>VLOOKUP(K60,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="11">
         <v>2</v>
       </c>
@@ -6423,21 +6493,22 @@
       <c r="Q61" s="13">
         <v>55</v>
       </c>
-      <c r="R61" s="12" t="s">
+      <c r="R61" s="13"/>
+      <c r="S61" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S61" s="16" t="s">
-        <v>346</v>
-      </c>
-      <c r="T61" t="e">
+      <c r="T61" s="16" t="s">
+        <v>345</v>
+      </c>
+      <c r="U61" t="e">
         <f>VLOOKUP(K61,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="X61" s="91" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y61" s="91" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="24">
         <v>1</v>
       </c>
@@ -6448,7 +6519,7 @@
         <v>148</v>
       </c>
       <c r="D62" s="25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E62" s="25" t="s">
         <v>179</v>
@@ -6489,19 +6560,20 @@
       <c r="Q62" s="77">
         <v>56</v>
       </c>
-      <c r="R62" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="S62" s="45"/>
-      <c r="T62" t="e">
+      <c r="R62" s="122"/>
+      <c r="S62" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="T62" s="45"/>
+      <c r="U62" t="e">
         <f>VLOOKUP(K62,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="X62" s="91" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y62" s="91" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="11">
         <v>2</v>
       </c>
@@ -6553,16 +6625,17 @@
       <c r="Q63" s="13">
         <v>57</v>
       </c>
-      <c r="R63" s="12" t="s">
+      <c r="R63" s="13"/>
+      <c r="S63" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S63" s="19"/>
-      <c r="T63" t="e">
+      <c r="T63" s="19"/>
+      <c r="U63" t="e">
         <f>VLOOKUP(K63,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="32">
         <v>3</v>
       </c>
@@ -6576,7 +6649,7 @@
         <v>263</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F64" s="12">
         <v>2</v>
@@ -6614,24 +6687,25 @@
       <c r="Q64" s="77">
         <v>58</v>
       </c>
-      <c r="R64" s="12" t="s">
+      <c r="R64" s="8"/>
+      <c r="S64" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S64" s="56" t="s">
-        <v>371</v>
-      </c>
-      <c r="T64" t="e">
+      <c r="T64" s="56" t="s">
+        <v>370</v>
+      </c>
+      <c r="U64" t="e">
         <f>VLOOKUP(K64,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U64" t="s">
-        <v>317</v>
-      </c>
-      <c r="X64" s="91" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V64" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y64" s="91" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A65" s="32">
         <v>2</v>
       </c>
@@ -6683,16 +6757,17 @@
       <c r="Q65" s="13">
         <v>59</v>
       </c>
-      <c r="R65" s="12" t="s">
+      <c r="R65" s="13"/>
+      <c r="S65" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="S65" s="16"/>
-      <c r="T65" t="e">
+      <c r="T65" s="16"/>
+      <c r="U65" t="e">
         <f>VLOOKUP(K65,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A66" s="11">
         <v>3</v>
       </c>
@@ -6706,7 +6781,7 @@
         <v>263</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F66" s="12">
         <v>2</v>
@@ -6744,24 +6819,25 @@
       <c r="Q66" s="77">
         <v>60</v>
       </c>
-      <c r="R66" s="12" t="s">
+      <c r="R66" s="8"/>
+      <c r="S66" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="S66" s="17" t="s">
-        <v>352</v>
-      </c>
-      <c r="T66" t="e">
+      <c r="T66" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="U66" t="e">
         <f>VLOOKUP(K66,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U66" t="s">
-        <v>317</v>
-      </c>
-      <c r="X66" s="91" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="V66" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y66" s="91" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A67" s="31">
         <v>1</v>
       </c>
@@ -6769,13 +6845,13 @@
         <v>2</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E67" s="63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F67" s="36">
         <v>2</v>
@@ -6813,49 +6889,50 @@
       <c r="Q67" s="13">
         <v>61</v>
       </c>
-      <c r="R67" s="58" t="s">
+      <c r="R67" s="13"/>
+      <c r="S67" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="S67" s="59" t="s">
-        <v>372</v>
-      </c>
-      <c r="T67" t="e">
+      <c r="T67" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="U67" t="e">
         <f>VLOOKUP(K67,datos!$B$2:$C$18,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="U67" t="s">
-        <v>312</v>
-      </c>
       <c r="V67" t="s">
-        <v>368</v>
-      </c>
-      <c r="W67">
+        <v>311</v>
+      </c>
+      <c r="W67" t="s">
+        <v>367</v>
+      </c>
+      <c r="X67">
         <v>20</v>
       </c>
-      <c r="X67" s="91" t="s">
-        <v>379</v>
+      <c r="Y67" s="91" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:S67" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R66">
+  <autoFilter ref="A5:T67" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S66">
       <sortCondition ref="K2:K64"/>
       <sortCondition ref="M2:M64"/>
       <sortCondition ref="A2:A64"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T64">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U64">
     <sortCondition ref="K2:K64"/>
     <sortCondition ref="M2:M64"/>
     <sortCondition ref="A2:A64"/>
     <sortCondition ref="F2:F64"/>
   </sortState>
   <mergeCells count="1">
-    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="S5:T5"/>
   </mergeCells>
-  <conditionalFormatting sqref="R10 R8:S9 R11:S33 R34 R35:S67 A7:N43 A6:J6 L6:S6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:Q67 Q7:S7 O7:P67">
+  <conditionalFormatting sqref="S10 S8:T9 S11:T33 S34 S35:T67 A7:N43 A6:J6 L6:T6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:R67 Q7:T7 O7:P67">
     <cfRule type="expression" dxfId="9" priority="18">
-      <formula>$T6=0</formula>
+      <formula>$U6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
@@ -6863,24 +6940,24 @@
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R6:R67">
+  <conditionalFormatting sqref="S6:S67">
     <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
     <cfRule type="expression" dxfId="6" priority="3">
-      <formula>$R6=0</formula>
+      <formula>$S6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
     <cfRule type="expression" dxfId="5" priority="2">
-      <formula>$R44=0</formula>
+      <formula>$S44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
     <cfRule type="expression" dxfId="4" priority="1">
-      <formula>$R58=0</formula>
+      <formula>$S58=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6893,7 +6970,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
   <dimension ref="B2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -6905,33 +6982,33 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="112" t="s">
-        <v>380</v>
-      </c>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="B2" s="113" t="s">
+        <v>379</v>
+      </c>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="112" t="s">
-        <v>388</v>
-      </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="B3" s="113" t="s">
+        <v>387</v>
+      </c>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="101" t="s">
+        <v>382</v>
+      </c>
+      <c r="C4" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="D4" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="D4" s="101" t="s">
-        <v>385</v>
-      </c>
       <c r="E4" s="102" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -6989,28 +7066,28 @@
       <c r="E9" s="85"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="118" t="s">
-        <v>381</v>
-      </c>
-      <c r="C11" s="119"/>
-      <c r="D11" s="120"/>
+      <c r="B11" s="119" t="s">
+        <v>380</v>
+      </c>
+      <c r="C11" s="120"/>
+      <c r="D11" s="121"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="115" t="s">
-        <v>396</v>
-      </c>
-      <c r="C12" s="116"/>
-      <c r="D12" s="117"/>
+      <c r="B12" s="116" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="117"/>
+      <c r="D12" s="118"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
+        <v>382</v>
+      </c>
+      <c r="C13" s="109" t="s">
         <v>383</v>
       </c>
-      <c r="C13" s="109" t="s">
-        <v>384</v>
-      </c>
       <c r="D13" s="107" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -7049,28 +7126,28 @@
       <c r="E19" s="110"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="112" t="s">
-        <v>382</v>
-      </c>
-      <c r="C20" s="112"/>
-      <c r="D20" s="112"/>
+      <c r="B20" s="113" t="s">
+        <v>381</v>
+      </c>
+      <c r="C20" s="113"/>
+      <c r="D20" s="113"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="112" t="s">
-        <v>389</v>
-      </c>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
+      <c r="B21" s="113" t="s">
+        <v>388</v>
+      </c>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
+        <v>385</v>
+      </c>
+      <c r="C22" s="104" t="s">
         <v>386</v>
       </c>
-      <c r="C22" s="104" t="s">
-        <v>387</v>
-      </c>
       <c r="D22" s="102" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -7101,28 +7178,28 @@
       <c r="D26" s="5"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="112" t="s">
-        <v>395</v>
-      </c>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
+      <c r="B28" s="113" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="112" t="s">
-        <v>390</v>
-      </c>
-      <c r="C29" s="112"/>
-      <c r="D29" s="112"/>
+      <c r="B29" s="113" t="s">
+        <v>389</v>
+      </c>
+      <c r="C29" s="113"/>
+      <c r="D29" s="113"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
+        <v>382</v>
+      </c>
+      <c r="C30" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="C30" s="101" t="s">
-        <v>384</v>
-      </c>
       <c r="D30" s="102" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
@@ -7148,28 +7225,28 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="114" t="s">
+      <c r="B35" s="115" t="s">
+        <v>390</v>
+      </c>
+      <c r="C35" s="115"/>
+      <c r="D35" s="115"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="114" t="s">
         <v>391</v>
       </c>
-      <c r="C35" s="114"/>
-      <c r="D35" s="114"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="113" t="s">
-        <v>392</v>
-      </c>
-      <c r="C36" s="113"/>
-      <c r="D36" s="113"/>
+      <c r="C36" s="114"/>
+      <c r="D36" s="114"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="101" t="s">
+        <v>392</v>
+      </c>
+      <c r="C37" s="101" t="s">
         <v>393</v>
       </c>
-      <c r="C37" s="101" t="s">
-        <v>394</v>
-      </c>
       <c r="D37" s="102" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -7191,33 +7268,33 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="121" t="s">
-        <v>400</v>
-      </c>
-      <c r="C41" s="121"/>
-      <c r="D41" s="121"/>
-      <c r="E41" s="121"/>
+      <c r="B41" s="112" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41" s="112"/>
+      <c r="D41" s="112"/>
+      <c r="E41" s="112"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="121" t="s">
-        <v>404</v>
-      </c>
-      <c r="C42" s="121"/>
-      <c r="D42" s="121"/>
-      <c r="E42" s="121"/>
+      <c r="B42" s="112" t="s">
+        <v>403</v>
+      </c>
+      <c r="C42" s="112"/>
+      <c r="D42" s="112"/>
+      <c r="E42" s="112"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C43" t="s">
+        <v>400</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>402</v>
-      </c>
       <c r="E43" s="36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
@@ -7231,7 +7308,7 @@
         <v>44364</v>
       </c>
       <c r="E44" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -7384,7 +7461,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -7395,7 +7472,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -7406,7 +7483,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -7417,7 +7494,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -7428,7 +7505,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -7439,7 +7516,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -7450,7 +7527,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -7461,7 +7538,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -7472,7 +7549,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -7483,7 +7560,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -7494,7 +7571,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B11">
         <v>3</v>
@@ -7505,7 +7582,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -7516,7 +7593,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B13">
         <v>3</v>
@@ -7527,7 +7604,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -7538,7 +7615,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -7549,7 +7626,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -7614,7 +7691,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -7623,13 +7700,13 @@
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>322</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>8</v>
@@ -7667,7 +7744,7 @@
         <v>61</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>21</v>
@@ -7708,7 +7785,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>136</v>
@@ -7717,7 +7794,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>136</v>
@@ -7749,7 +7826,7 @@
         <v>116</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>136</v>
@@ -7788,7 +7865,7 @@
         <v>92</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>136</v>
@@ -7797,7 +7874,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M5" s="3" t="s">
         <v>21</v>
@@ -7810,7 +7887,7 @@
         <v>36</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -7833,7 +7910,7 @@
         <v>15</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>136</v>
@@ -7872,7 +7949,7 @@
         <v>91</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>136</v>
@@ -7909,7 +7986,7 @@
         <v>57</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>21</v>
@@ -7952,7 +8029,7 @@
         <v>85</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>21</v>
@@ -7995,7 +8072,7 @@
         <v>64</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>21</v>
@@ -8038,7 +8115,7 @@
         <v>68</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>21</v>
@@ -8081,7 +8158,7 @@
         <v>82</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>30</v>
@@ -8115,16 +8192,16 @@
         <v>44235.345856481501</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>328</v>
-      </c>
       <c r="G13" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>21</v>
@@ -8137,7 +8214,7 @@
         <v>34</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>30</v>
@@ -8150,7 +8227,7 @@
         <v>24</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -8173,7 +8250,7 @@
         <v>132</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>21</v>
@@ -8188,7 +8265,7 @@
         <v>36</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>30</v>
@@ -8224,7 +8301,7 @@
         <v>113</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>30</v>
@@ -8267,7 +8344,7 @@
         <v>27</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>21</v>
@@ -8280,7 +8357,7 @@
         <v>29</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M16" s="3" t="s">
         <v>30</v>
@@ -8314,7 +8391,7 @@
         <v>101</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>30</v>
@@ -8357,7 +8434,7 @@
         <v>20</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>21</v>
@@ -8400,7 +8477,7 @@
         <v>79</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>21</v>
@@ -8443,7 +8520,7 @@
         <v>79</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>30</v>
@@ -8486,7 +8563,7 @@
         <v>120</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>21</v>
@@ -8499,7 +8576,7 @@
         <v>29</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M21" s="3" t="s">
         <v>30</v>
@@ -8535,7 +8612,7 @@
         <v>33</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>21</v>
@@ -8550,7 +8627,7 @@
         <v>34</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M22" s="3" t="s">
         <v>30</v>
@@ -8559,7 +8636,7 @@
         <v>22</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P22" s="2" t="s">
         <v>36</v>
@@ -8588,7 +8665,7 @@
         <v>108</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>21</v>
@@ -8603,7 +8680,7 @@
         <v>34</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M23" s="3" t="s">
         <v>30</v>
@@ -8612,13 +8689,13 @@
         <v>22</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P23" s="2" t="s">
         <v>36</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -8641,7 +8718,7 @@
         <v>105</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>21</v>
@@ -8654,7 +8731,7 @@
         <v>76</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M24" s="3" t="s">
         <v>30</v>
@@ -8667,7 +8744,7 @@
         <v>24</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -8690,7 +8767,7 @@
         <v>88</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>21</v>
@@ -8733,7 +8810,7 @@
         <v>74</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>21</v>
@@ -8748,7 +8825,7 @@
         <v>36</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M26" s="3" t="s">
         <v>30</v>
@@ -8782,7 +8859,7 @@
         <v>124</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H27" s="3" t="s">
         <v>136</v>
@@ -8821,7 +8898,7 @@
         <v>54</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>21</v>
@@ -8834,7 +8911,7 @@
         <v>29</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M28" s="3" t="s">
         <v>136</v>
@@ -8843,7 +8920,7 @@
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -8866,7 +8943,7 @@
         <v>40</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H29" s="3" t="s">
         <v>30</v>
@@ -8888,7 +8965,7 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -8911,7 +8988,7 @@
         <v>40</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>21</v>
@@ -8926,7 +9003,7 @@
         <v>76</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M30" s="3" t="s">
         <v>30</v>
@@ -8941,7 +9018,7 @@
         <v>24</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
@@ -8964,7 +9041,7 @@
         <v>99</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>21</v>
@@ -8979,7 +9056,7 @@
         <v>76</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M31" s="3" t="s">
         <v>30</v>
@@ -9015,7 +9092,7 @@
         <v>50</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>21</v>
@@ -9058,7 +9135,7 @@
         <v>95</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>21</v>
@@ -9101,7 +9178,7 @@
         <v>128</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>21</v>
@@ -9302,13 +9379,13 @@
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>349</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>350</v>
       </c>
       <c r="H2">
         <v>71</v>
@@ -9398,7 +9475,7 @@
         <v/>
       </c>
       <c r="J5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="L5" t="str">
         <f>H19&amp;", "&amp;H20&amp;", "&amp;H21&amp;", "&amp;H22&amp;", "&amp;H23&amp;", "&amp;H24&amp;", "&amp;H25&amp;", "&amp;H26&amp;", "&amp;H27&amp;", "&amp;H28&amp;", "&amp;H29&amp;", "&amp;H30</f>
@@ -9428,7 +9505,7 @@
         <v/>
       </c>
       <c r="J6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -9465,7 +9542,7 @@
         <v/>
       </c>
       <c r="C8" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D8">
         <v>10</v>
@@ -9602,7 +9679,7 @@
         <v/>
       </c>
       <c r="J13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -9628,7 +9705,7 @@
         <v/>
       </c>
       <c r="J14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -9948,25 +10025,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I1" s="52">
         <v>0.125</v>
@@ -9998,7 +10075,7 @@
         <v>"Trabajo de Repositorios de Información"</v>
       </c>
       <c r="G2" t="str">
-        <f>""""&amp;IF(OR(planificación!R6="online",planificación!R6="polideportivo",planificación!R6="entrega"),planificación!R6,planificación!S6)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S6="online",planificación!S6="polideportivo",planificación!S6="entrega"),planificación!S6,planificación!T6)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10028,7 +10105,7 @@
         <v>"Examen Teórico de Sistemas Operativos"</v>
       </c>
       <c r="G3" t="str">
-        <f>""""&amp;IF(OR(planificación!R7="online",planificación!R7="polideportivo",planificación!R7="entrega"),planificación!R7,planificación!S7)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S7="online",planificación!S7="polideportivo",planificación!S7="entrega"),planificación!S7,planificación!T7)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10058,7 +10135,7 @@
         <v>"Examen Teórico de Diseño del Software"</v>
       </c>
       <c r="G4" t="str">
-        <f>""""&amp;IF(OR(planificación!R8="online",planificación!R8="polideportivo",planificación!R8="entrega"),planificación!R8,planificación!S8)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S8="online",planificación!S8="polideportivo",planificación!S8="entrega"),planificación!S8,planificación!T8)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -10088,7 +10165,7 @@
         <v>"Trabajo de Software para Dispositivos Móviles"</v>
       </c>
       <c r="G5" t="str">
-        <f>""""&amp;IF(OR(planificación!R9="online",planificación!R9="polideportivo",planificación!R9="entrega"),planificación!R9,planificación!S9)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S9="online",planificación!S9="polideportivo",planificación!S9="entrega"),planificación!S9,planificación!T9)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -10118,7 +10195,7 @@
         <v>"Examen Teórico de Arquitectura de Computadores"</v>
       </c>
       <c r="G6" t="str">
-        <f>""""&amp;IF(OR(planificación!R10="online",planificación!R10="polideportivo",planificación!R10="entrega"),planificación!R10,planificación!S10)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S10="online",planificación!S10="polideportivo",planificación!S10="entrega"),planificación!S10,planificación!T10)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10148,14 +10225,14 @@
         <v>"Trabajo de Administración de Sistemas y Redes"</v>
       </c>
       <c r="G7" t="str">
-        <f>""""&amp;IF(OR(planificación!R11="online",planificación!R11="polideportivo",planificación!R11="entrega"),planificación!R11,planificación!S11)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S11="online",planificación!S11="polideportivo",planificación!S11="entrega"),planificación!S11,planificación!T11)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE("""",planificación!D12," ",planificación!G12,"""")</f>
-        <v>"SI Teórico"</v>
+        <v>" Teórico"</v>
       </c>
       <c r="B8" s="30">
         <f>planificación!K12</f>
@@ -10178,7 +10255,7 @@
         <v>"Examen Teórico de Sistemas Inteligentes"</v>
       </c>
       <c r="G8" t="str">
-        <f>""""&amp;IF(OR(planificación!R12="online",planificación!R12="polideportivo",planificación!R12="entrega"),planificación!R12,planificación!S12)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S12="online",planificación!S12="polideportivo",planificación!S12="entrega"),planificación!S12,planificación!T12)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -10208,14 +10285,14 @@
         <v>"Examen Práctico de Tecnología y Paradigmas de Programación"</v>
       </c>
       <c r="G9" t="str">
-        <f>""""&amp;IF(OR(planificación!R13="online",planificación!R13="polideportivo",planificación!R13="entrega"),planificación!R13,planificación!S13)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S13="online",planificación!S13="polideportivo",planificación!S13="entrega"),planificación!S13,planificación!T13)&amp;""""</f>
         <v>"L-14, L-31, L-32,  L-11"</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE("""",planificación!D14," ",planificación!G14,"""")</f>
-        <v>"FI Teórico"</v>
+        <v>"FI "</v>
       </c>
       <c r="B10" s="30">
         <f>planificación!K14</f>
@@ -10235,10 +10312,10 @@
       </c>
       <c r="F10" t="str">
         <f>CONCATENATE(IF(planificación!G14&lt;&gt;"trabajo",CONCATENATE("""Examen ",planificación!G14),""""&amp;"Trabajo")&amp;" de ",planificación!E14,"""")</f>
-        <v>"Examen Teórico de Fundamentos de Informática"</v>
+        <v>"Examen  de Fundamentos de Informática"</v>
       </c>
       <c r="G10" t="str">
-        <f>""""&amp;IF(OR(planificación!R14="online",planificación!R14="polideportivo",planificación!R14="entrega"),planificación!R14,planificación!S14)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S14="online",planificación!S14="polideportivo",planificación!S14="entrega"),planificación!S14,planificación!T14)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10268,7 +10345,7 @@
         <v>"Examen Teórico de Repositorios de Información"</v>
       </c>
       <c r="G11" t="str">
-        <f>""""&amp;IF(OR(planificación!R15="online",planificación!R15="polideportivo",planificación!R15="entrega"),planificación!R15,planificación!S15)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S15="online",planificación!S15="polideportivo",planificación!S15="entrega"),planificación!S15,planificación!T15)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10298,7 +10375,7 @@
         <v>"Examen Teórico de Ingeniería de Requisitos"</v>
       </c>
       <c r="G12" t="str">
-        <f>""""&amp;IF(OR(planificación!R16="online",planificación!R16="polideportivo",planificación!R16="entrega"),planificación!R16,planificación!S16)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S16="online",planificación!S16="polideportivo",planificación!S16="entrega"),planificación!S16,planificación!T16)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10328,7 +10405,7 @@
         <v>"Examen Teórico de Ingeniería del Proceso Software"</v>
       </c>
       <c r="G13" t="str">
-        <f>""""&amp;IF(OR(planificación!R17="online",planificación!R17="polideportivo",planificación!R17="entrega"),planificación!R17,planificación!S17)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S17="online",planificación!S17="polideportivo",planificación!S17="entrega"),planificación!S17,planificación!T17)&amp;""""</f>
         <v>"A-B-01, A-B-02"</v>
       </c>
     </row>
@@ -10358,7 +10435,7 @@
         <v>"Examen Teórico de Estructura de Datos"</v>
       </c>
       <c r="G14" t="str">
-        <f>""""&amp;IF(OR(planificación!R18="online",planificación!R18="polideportivo",planificación!R18="entrega"),planificación!R18,planificación!S18)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S18="online",planificación!S18="polideportivo",planificación!S18="entrega"),planificación!S18,planificación!T18)&amp;""""</f>
         <v>"A-S-01, A-S-02"</v>
       </c>
     </row>
@@ -10388,7 +10465,7 @@
         <v>"Trabajo de Software para Dispositivos Móviles"</v>
       </c>
       <c r="G15" t="str">
-        <f>""""&amp;IF(OR(planificación!R19="online",planificación!R19="polideportivo",planificación!R19="entrega"),planificación!R19,planificación!S19)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S19="online",planificación!S19="polideportivo",planificación!S19="entrega"),planificación!S19,planificación!T19)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -10418,7 +10495,7 @@
         <v>"Examen Teórico de "</v>
       </c>
       <c r="G16" t="str">
-        <f>""""&amp;IF(OR(planificación!R20="online",planificación!R20="polideportivo",planificación!R20="entrega"),planificación!R20,planificación!S20)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S20="online",planificación!S20="polideportivo",planificación!S20="entrega"),planificación!S20,planificación!T20)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10448,7 +10525,7 @@
         <v>"Examen Teórico de Sistemas Distribuidos e Internet"</v>
       </c>
       <c r="G17" t="str">
-        <f>""""&amp;IF(OR(planificación!R21="online",planificación!R21="polideportivo",planificación!R21="entrega"),planificación!R21,planificación!S21)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S21="online",planificación!S21="polideportivo",planificación!S21="entrega"),planificación!S21,planificación!T21)&amp;""""</f>
         <v>"A-S-01, A-S-02"</v>
       </c>
     </row>
@@ -10478,7 +10555,7 @@
         <v>"Examen Teórico de Comunicación Persona-Máquina"</v>
       </c>
       <c r="G18" t="str">
-        <f>""""&amp;IF(OR(planificación!R22="online",planificación!R22="polideportivo",planificación!R22="entrega"),planificación!R22,planificación!S22)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S22="online",planificación!S22="polideportivo",planificación!S22="entrega"),planificación!S22,planificación!T22)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10508,7 +10585,7 @@
         <v>"Examen Práctico de Metodología de la Programación"</v>
       </c>
       <c r="G19" t="str">
-        <f>""""&amp;IF(OR(planificación!R23="online",planificación!R23="polideportivo",planificación!R23="entrega"),planificación!R23,planificación!S23)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S23="online",planificación!S23="polideportivo",planificación!S23="entrega"),planificación!S23,planificación!T23)&amp;""""</f>
         <v>"L-14, L-31, L-32"</v>
       </c>
     </row>
@@ -10538,7 +10615,7 @@
         <v>"Examen Teórico de Computación Numérica"</v>
       </c>
       <c r="G20" t="str">
-        <f>""""&amp;IF(OR(planificación!R24="online",planificación!R24="polideportivo",planificación!R24="entrega"),planificación!R24,planificación!S24)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S24="online",planificación!S24="polideportivo",planificación!S24="entrega"),planificación!S24,planificación!T24)&amp;""""</f>
         <v>"A-2-01"</v>
       </c>
     </row>
@@ -10568,7 +10645,7 @@
         <v>"Examen Teórico de Sistemas de Información para la Web"</v>
       </c>
       <c r="G21" t="str">
-        <f>""""&amp;IF(OR(planificación!R25="online",planificación!R25="polideportivo",planificación!R25="entrega"),planificación!R25,planificación!S25)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S25="online",planificación!S25="polideportivo",planificación!S25="entrega"),planificación!S25,planificación!T25)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10598,7 +10675,7 @@
         <v>"Trabajo de Sistemas de Información para la Web"</v>
       </c>
       <c r="G22" t="str">
-        <f>""""&amp;IF(OR(planificación!R26="online",planificación!R26="polideportivo",planificación!R26="entrega"),planificación!R26,planificación!S26)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S26="online",planificación!S26="polideportivo",planificación!S26="entrega"),planificación!S26,planificación!T26)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -10628,7 +10705,7 @@
         <v>"Examen Teórico de Arquitectura del Software"</v>
       </c>
       <c r="G23" t="str">
-        <f>""""&amp;IF(OR(planificación!R27="online",planificación!R27="polideportivo",planificación!R27="entrega"),planificación!R27,planificación!S27)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S27="online",planificación!S27="polideportivo",planificación!S27="entrega"),planificación!S27,planificación!T27)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10658,7 +10735,7 @@
         <v>"Trabajo de Arquitectura del Software"</v>
       </c>
       <c r="G24" t="str">
-        <f>""""&amp;IF(OR(planificación!R28="online",planificación!R28="polideportivo",planificación!R28="entrega"),planificación!R28,planificación!S28)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S28="online",planificación!S28="polideportivo",planificación!S28="entrega"),planificación!S28,planificación!T28)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10688,7 +10765,7 @@
         <v>"Examen Teórico de Fundamentos de Computadores y Redes"</v>
       </c>
       <c r="G25" t="str">
-        <f>""""&amp;IF(OR(planificación!R29="online",planificación!R29="polideportivo",planificación!R29="entrega"),planificación!R29,planificación!S29)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S29="online",planificación!S29="polideportivo",planificación!S29="entrega"),planificación!S29,planificación!T29)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -10718,7 +10795,7 @@
         <v>"Examen Teórico de Algoritmia"</v>
       </c>
       <c r="G26" t="str">
-        <f>""""&amp;IF(OR(planificación!R30="online",planificación!R30="polideportivo",planificación!R30="entrega"),planificación!R30,planificación!S30)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S30="online",planificación!S30="polideportivo",planificación!S30="entrega"),planificación!S30,planificación!T30)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -10748,7 +10825,7 @@
         <v>"Examen Teórico de Integración de aplicaciones empresariales"</v>
       </c>
       <c r="G27" t="str">
-        <f>""""&amp;IF(OR(planificación!R31="online",planificación!R31="polideportivo",planificación!R31="entrega"),planificación!R31,planificación!S31)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S31="online",planificación!S31="polideportivo",planificación!S31="entrega"),planificación!S31,planificación!T31)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -10778,7 +10855,7 @@
         <v>"Examen Teórico de Ondas y Electromagnetismo"</v>
       </c>
       <c r="G28" t="str">
-        <f>""""&amp;IF(OR(planificación!R32="online",planificación!R32="polideportivo",planificación!R32="entrega"),planificación!R32,planificación!S32)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S32="online",planificación!S32="polideportivo",planificación!S32="entrega"),planificación!S32,planificación!T32)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -10808,7 +10885,7 @@
         <v>"Examen Teórico de Seguridad de Sistemas Informáticos"</v>
       </c>
       <c r="G29" t="str">
-        <f>""""&amp;IF(OR(planificación!R33="online",planificación!R33="polideportivo",planificación!R33="entrega"),planificación!R33,planificación!S33)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S33="online",planificación!S33="polideportivo",planificación!S33="entrega"),planificación!S33,planificación!T33)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -10838,7 +10915,7 @@
         <v>"Examen Práctico de Arquitectura de Computadores"</v>
       </c>
       <c r="G30" t="str">
-        <f>""""&amp;IF(OR(planificación!R34="online",planificación!R34="polideportivo",planificación!R34="entrega"),planificación!R34,planificación!S34)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S34="online",planificación!S34="polideportivo",planificación!S34="entrega"),planificación!S34,planificación!T34)&amp;""""</f>
         <v>"L-11, L-12, L-13, L-14, L-15, L-04"</v>
       </c>
     </row>
@@ -10868,7 +10945,7 @@
         <v>"Examen Práctico de Fundamentos de Informática (80)"</v>
       </c>
       <c r="G31" t="str">
-        <f>""""&amp;IF(OR(planificación!R35="online",planificación!R35="polideportivo",planificación!R35="entrega"),planificación!R35,planificación!S35)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S35="online",planificación!S35="polideportivo",planificación!S35="entrega"),planificación!S35,planificación!T35)&amp;""""</f>
         <v>"L-14, L-31, L-32, L-11, L-12, L-13"</v>
       </c>
     </row>
@@ -10898,7 +10975,7 @@
         <v>"Examen Teórico de Calidad, Validación y Verificación del Software"</v>
       </c>
       <c r="G32" t="str">
-        <f>""""&amp;IF(OR(planificación!R36="online",planificación!R36="polideportivo",planificación!R36="entrega"),planificación!R36,planificación!S36)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S36="online",planificación!S36="polideportivo",planificación!S36="entrega"),planificación!S36,planificación!T36)&amp;""""</f>
         <v>"A-2-01"</v>
       </c>
     </row>
@@ -10928,7 +11005,7 @@
         <v>"Examen Práctico de Sistemas Operativos"</v>
       </c>
       <c r="G33" t="str">
-        <f>""""&amp;IF(OR(planificación!R37="online",planificación!R37="polideportivo",planificación!R37="entrega"),planificación!R37,planificación!S37)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S37="online",planificación!S37="polideportivo",planificación!S37="entrega"),planificación!S37,planificación!T37)&amp;""""</f>
         <v>"L-04, L-01, L-02, L-03, L-05, "</v>
       </c>
     </row>
@@ -10958,7 +11035,7 @@
         <v>"Examen Práctico de Autómatas y Matemáticas Discretas"</v>
       </c>
       <c r="G34" t="str">
-        <f>""""&amp;IF(OR(planificación!R38="online",planificación!R38="polideportivo",planificación!R38="entrega"),planificación!R38,planificación!S38)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S38="online",planificación!S38="polideportivo",planificación!S38="entrega"),planificación!S38,planificación!T38)&amp;""""</f>
         <v>"L-11, L-12, L-13, L-14, L-15, L-04, L-03"</v>
       </c>
     </row>
@@ -10988,7 +11065,7 @@
         <v>"Examen Teórico de Software y Estándares para la Web"</v>
       </c>
       <c r="G35" t="str">
-        <f>""""&amp;IF(OR(planificación!R39="online",planificación!R39="polideportivo",planificación!R39="entrega"),planificación!R39,planificación!S39)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S39="online",planificación!S39="polideportivo",planificación!S39="entrega"),planificación!S39,planificación!T39)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11018,7 +11095,7 @@
         <v>"Trabajo de Software y Estándares para la Web"</v>
       </c>
       <c r="G36" t="str">
-        <f>""""&amp;IF(OR(planificación!R40="online",planificación!R40="polideportivo",planificación!R40="entrega"),planificación!R40,planificación!S40)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S40="online",planificación!S40="polideportivo",planificación!S40="entrega"),planificación!S40,planificación!T40)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11048,7 +11125,7 @@
         <v>"Examen Práctico de Estructura de Datos"</v>
       </c>
       <c r="G37" t="str">
-        <f>""""&amp;IF(OR(planificación!R41="online",planificación!R41="polideportivo",planificación!R41="entrega"),planificación!R41,planificación!S41)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S41="online",planificación!S41="polideportivo",planificación!S41="entrega"),planificación!S41,planificación!T41)&amp;""""</f>
         <v>"L-14, L-04, L-12, L-13, L-15, L-16"</v>
       </c>
     </row>
@@ -11078,7 +11155,7 @@
         <v>"Trabajo de Informática Audiovisual"</v>
       </c>
       <c r="G38" t="str">
-        <f>""""&amp;IF(OR(planificación!R42="online",planificación!R42="polideportivo",planificación!R42="entrega"),planificación!R42,planificación!S42)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S42="online",planificación!S42="polideportivo",planificación!S42="entrega"),planificación!S42,planificación!T42)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -11108,7 +11185,7 @@
         <v>"Examen Práctico de Diseño del Software"</v>
       </c>
       <c r="G39" t="str">
-        <f>""""&amp;IF(OR(planificación!R43="online",planificación!R43="polideportivo",planificación!R43="entrega"),planificación!R43,planificación!S43)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S43="online",planificación!S43="polideportivo",planificación!S43="entrega"),planificación!S43,planificación!T43)&amp;""""</f>
         <v>"L-14, L-31, L-32, L-11, L-12, L-13"</v>
       </c>
     </row>
@@ -11138,7 +11215,7 @@
         <v>"Examen Teórico de Empresa"</v>
       </c>
       <c r="G40" t="str">
-        <f>""""&amp;IF(OR(planificación!R44="online",planificación!R44="polideportivo",planificación!R44="entrega"),planificación!R44,planificación!S44)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S44="online",planificación!S44="polideportivo",planificación!S44="entrega"),planificación!S44,planificación!T44)&amp;""""</f>
         <v>"A-S-01, A-S-02"</v>
       </c>
     </row>
@@ -11168,7 +11245,7 @@
         <v>"Examen Teórico de Bases de Datos"</v>
       </c>
       <c r="G41" t="str">
-        <f>""""&amp;IF(OR(planificación!R45="online",planificación!R45="polideportivo",planificación!R45="entrega"),planificación!R45,planificación!S45)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S45="online",planificación!S45="polideportivo",planificación!S45="entrega"),planificación!S45,planificación!T45)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -11198,7 +11275,7 @@
         <v>"Examen Teórico de Cálculo"</v>
       </c>
       <c r="G42" t="str">
-        <f>""""&amp;IF(OR(planificación!R46="online",planificación!R46="polideportivo",planificación!R46="entrega"),planificación!R46,planificación!S46)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S46="online",planificación!S46="polideportivo",planificación!S46="entrega"),planificación!S46,planificación!T46)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -11228,7 +11305,7 @@
         <v>"Examen Teórico de Informática Forense y Auditoría"</v>
       </c>
       <c r="G43" t="str">
-        <f>""""&amp;IF(OR(planificación!R47="online",planificación!R47="polideportivo",planificación!R47="entrega"),planificación!R47,planificación!S47)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S47="online",planificación!S47="polideportivo",planificación!S47="entrega"),planificación!S47,planificación!T47)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11258,7 +11335,7 @@
         <v>"Examen Práctico de Comunicación Persona-Máquina"</v>
       </c>
       <c r="G44" t="str">
-        <f>""""&amp;IF(OR(planificación!R48="online",planificación!R48="polideportivo",planificación!R48="entrega"),planificación!R48,planificación!S48)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S48="online",planificación!S48="polideportivo",planificación!S48="entrega"),planificación!S48,planificación!T48)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11288,7 +11365,7 @@
         <v>"Trabajo de Software y Estándares para la Web"</v>
       </c>
       <c r="G45" t="str">
-        <f>""""&amp;IF(OR(planificación!R49="online",planificación!R49="polideportivo",planificación!R49="entrega"),planificación!R49,planificación!S49)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S49="online",planificación!S49="polideportivo",planificación!S49="entrega"),planificación!S49,planificación!T49)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11318,7 +11395,7 @@
         <v>"Examen Práctico de Introducción a la Programación"</v>
       </c>
       <c r="G46" t="str">
-        <f>""""&amp;IF(OR(planificación!R50="online",planificación!R50="polideportivo",planificación!R50="entrega"),planificación!R50,planificación!S50)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S50="online",planificación!S50="polideportivo",planificación!S50="entrega"),planificación!S50,planificación!T50)&amp;""""</f>
         <v>"L-14, L-31, L-32, "</v>
       </c>
     </row>
@@ -11348,7 +11425,7 @@
         <v>"Examen Teórico de Dirección y Planificación de Proyectos Informáticos"</v>
       </c>
       <c r="G47" t="str">
-        <f>""""&amp;IF(OR(planificación!R51="online",planificación!R51="polideportivo",planificación!R51="entrega"),planificación!R51,planificación!S51)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S51="online",planificación!S51="polideportivo",planificación!S51="entrega"),planificación!S51,planificación!T51)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11378,7 +11455,7 @@
         <v>"Examen Práctico de Algoritmia"</v>
       </c>
       <c r="G48" t="str">
-        <f>""""&amp;IF(OR(planificación!R52="online",planificación!R52="polideportivo",planificación!R52="entrega"),planificación!R52,planificación!S52)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S52="online",planificación!S52="polideportivo",planificación!S52="entrega"),planificación!S52,planificación!T52)&amp;""""</f>
         <v>"L-11, L-12, L-13, "</v>
       </c>
     </row>
@@ -11408,7 +11485,7 @@
         <v>"Examen Teórico de Estadística"</v>
       </c>
       <c r="G49" t="str">
-        <f>""""&amp;IF(OR(planificación!R53="online",planificación!R53="polideportivo",planificación!R53="entrega"),planificación!R53,planificación!S53)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S53="online",planificación!S53="polideportivo",planificación!S53="entrega"),planificación!S53,planificación!T53)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -11438,7 +11515,7 @@
         <v>"Examen Práctico de Sistemas Distribuidos e Internet"</v>
       </c>
       <c r="G50" t="str">
-        <f>""""&amp;IF(OR(planificación!R54="online",planificación!R54="polideportivo",planificación!R54="entrega"),planificación!R54,planificación!S54)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S54="online",planificación!S54="polideportivo",planificación!S54="entrega"),planificación!S54,planificación!T54)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11468,7 +11545,7 @@
         <v>"Examen Práctico de Computación Numérica"</v>
       </c>
       <c r="G51" t="str">
-        <f>""""&amp;IF(OR(planificación!R55="online",planificación!R55="polideportivo",planificación!R55="entrega"),planificación!R55,planificación!S55)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S55="online",planificación!S55="polideportivo",planificación!S55="entrega"),planificación!S55,planificación!T55)&amp;""""</f>
         <v>"L-14, L-31, L-32"</v>
       </c>
     </row>
@@ -11498,7 +11575,7 @@
         <v>"Trabajo de Software para Robots"</v>
       </c>
       <c r="G52" t="str">
-        <f>""""&amp;IF(OR(planificación!R56="online",planificación!R56="polideportivo",planificación!R56="entrega"),planificación!R56,planificación!S56)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S56="online",planificación!S56="polideportivo",planificación!S56="entrega"),planificación!S56,planificación!T56)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -11528,7 +11605,7 @@
         <v>"Examen Práctico de Seguridad de Sistemas Informáticos"</v>
       </c>
       <c r="G53" t="str">
-        <f>""""&amp;IF(OR(planificación!R57="online",planificación!R57="polideportivo",planificación!R57="entrega"),planificación!R57,planificación!S57)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S57="online",planificación!S57="polideportivo",planificación!S57="entrega"),planificación!S57,planificación!T57)&amp;""""</f>
         <v>"L-14, L-31, L-32, L-11, L-12, "</v>
       </c>
     </row>
@@ -11558,7 +11635,7 @@
         <v>"Examen Teórico de Computabilidad"</v>
       </c>
       <c r="G54" t="str">
-        <f>""""&amp;IF(OR(planificación!R58="online",planificación!R58="polideportivo",planificación!R58="entrega"),planificación!R58,planificación!S58)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S58="online",planificación!S58="polideportivo",planificación!S58="entrega"),planificación!S58,planificación!T58)&amp;""""</f>
         <v>"A-2-01, A-2-02"</v>
       </c>
     </row>
@@ -11588,7 +11665,7 @@
         <v>"Examen Teórico de Aspectos Sociales, Legales, Éticos y Prof. de la Informática"</v>
       </c>
       <c r="G55" t="str">
-        <f>""""&amp;IF(OR(planificación!R59="online",planificación!R59="polideportivo",planificación!R59="entrega"),planificación!R59,planificación!S59)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S59="online",planificación!S59="polideportivo",planificación!S59="entrega"),planificación!S59,planificación!T59)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11618,7 +11695,7 @@
         <v>"Trabajo de Software de entretenimiento y videojuegos"</v>
       </c>
       <c r="G56" t="str">
-        <f>""""&amp;IF(OR(planificación!R60="online",planificación!R60="polideportivo",planificación!R60="entrega"),planificación!R60,planificación!S60)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S60="online",planificación!S60="polideportivo",planificación!S60="entrega"),planificación!S60,planificación!T60)&amp;""""</f>
         <v>"entrega"</v>
       </c>
     </row>
@@ -11648,7 +11725,7 @@
         <v>"Examen Práctico de Bases de Datos"</v>
       </c>
       <c r="G57" t="str">
-        <f>""""&amp;IF(OR(planificación!R61="online",planificación!R61="polideportivo",planificación!R61="entrega"),planificación!R61,planificación!S61)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S61="online",planificación!S61="polideportivo",planificación!S61="entrega"),planificación!S61,planificación!T61)&amp;""""</f>
         <v>"L-14, L-31, L-32, L-11, L-04, "</v>
       </c>
     </row>
@@ -11678,7 +11755,7 @@
         <v>"Examen Teórico de Álgebra Lineal"</v>
       </c>
       <c r="G58" t="str">
-        <f>""""&amp;IF(OR(planificación!R62="online",planificación!R62="polideportivo",planificación!R62="entrega"),planificación!R62,planificación!S62)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S62="online",planificación!S62="polideportivo",planificación!S62="entrega"),planificación!S62,planificación!T62)&amp;""""</f>
         <v>"polideportivo"</v>
       </c>
     </row>
@@ -11708,7 +11785,7 @@
         <v>"Examen Teórico de Tecnología Electrónica de Computadores"</v>
       </c>
       <c r="G59" t="str">
-        <f>""""&amp;IF(OR(planificación!R63="online",planificación!R63="polideportivo",planificación!R63="entrega"),planificación!R63,planificación!S63)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S63="online",planificación!S63="polideportivo",planificación!S63="entrega"),planificación!S63,planificación!T63)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11738,7 +11815,7 @@
         <v>"Examen Práctico de Diseño de Lenguajes de Programación 100 (tanda 1)"</v>
       </c>
       <c r="G60" t="str">
-        <f>""""&amp;IF(OR(planificación!R64="online",planificación!R64="polideportivo",planificación!R64="entrega"),planificación!R64,planificación!S64)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S64="online",planificación!S64="polideportivo",planificación!S64="entrega"),planificación!S64,planificación!T64)&amp;""""</f>
         <v>"L-14, L-31, L-32, L-11, L-04, L-01, L-15"</v>
       </c>
     </row>
@@ -11768,7 +11845,7 @@
         <v>"Examen Práctico de Tecnología Electrónica de Computadores"</v>
       </c>
       <c r="G61" t="str">
-        <f>""""&amp;IF(OR(planificación!R65="online",planificación!R65="polideportivo",planificación!R65="entrega"),planificación!R65,planificación!S65)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S65="online",planificación!S65="polideportivo",planificación!S65="entrega"),planificación!S65,planificación!T65)&amp;""""</f>
         <v>"online"</v>
       </c>
     </row>
@@ -11798,7 +11875,7 @@
         <v>"Examen Práctico de Diseño de Lenguajes de Programación 100 (tanda 2)"</v>
       </c>
       <c r="G62" t="str">
-        <f>""""&amp;IF(OR(planificación!R66="online",planificación!R66="polideportivo",planificación!R66="entrega"),planificación!R66,planificación!S66)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S66="online",planificación!S66="polideportivo",planificación!S66="entrega"),planificación!S66,planificación!T66)&amp;""""</f>
         <v>"L-12, L-13"</v>
       </c>
     </row>
@@ -11828,7 +11905,7 @@
         <v>"Examen Práctico de Fundamentos de Computadores y Redes"</v>
       </c>
       <c r="G63" t="str">
-        <f>""""&amp;IF(OR(planificación!R67="online",planificación!R67="polideportivo",planificación!R67="entrega"),planificación!R67,planificación!S67)&amp;""""</f>
+        <f>""""&amp;IF(OR(planificación!S67="online",planificación!S67="polideportivo",planificación!S67="entrega"),planificación!S67,planificación!T67)&amp;""""</f>
         <v>"L-13, L-15, L-14"</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Each day can now be configured a different Interval for the exams.
Needs to be solved little issue involving rounding.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE2D22F-C7B0-4887-9617-1F39F3645847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006BA216-9943-496B-88CE-E9FD57095D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="26430" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="26430" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -2029,6 +2029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2062,12 +2063,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2144,57 +2195,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2221,23 +2221,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="21"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="12"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2542,8 +2542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2650,10 +2650,10 @@
       <c r="R5" s="92" t="s">
         <v>404</v>
       </c>
-      <c r="S5" s="111" t="s">
+      <c r="S5" s="112" t="s">
         <v>298</v>
       </c>
-      <c r="T5" s="111"/>
+      <c r="T5" s="112"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -3819,7 +3819,7 @@
       <c r="Q22" s="77">
         <v>16</v>
       </c>
-      <c r="R22" s="122"/>
+      <c r="R22" s="111"/>
       <c r="S22" s="65" t="s">
         <v>253</v>
       </c>
@@ -6560,7 +6560,7 @@
       <c r="Q62" s="77">
         <v>56</v>
       </c>
-      <c r="R62" s="122"/>
+      <c r="R62" s="111"/>
       <c r="S62" s="25" t="s">
         <v>297</v>
       </c>
@@ -6931,32 +6931,32 @@
     <mergeCell ref="S5:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="S10 S8:T9 S11:T33 S34 S35:T67 A7:N43 A6:J6 L6:T6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:R67 Q7:T7 O7:P67">
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>$U6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S67">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="23" priority="3">
       <formula>$S6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>$S44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>$S58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6982,20 +6982,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="114" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="114" t="s">
         <v>387</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="113"/>
+      <c r="C3" s="114"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="101" t="s">
@@ -7066,18 +7066,18 @@
       <c r="E9" s="85"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="119" t="s">
+      <c r="B11" s="120" t="s">
         <v>380</v>
       </c>
-      <c r="C11" s="120"/>
-      <c r="D11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="122"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="117" t="s">
         <v>395</v>
       </c>
-      <c r="C12" s="117"/>
-      <c r="D12" s="118"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="119"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -7126,18 +7126,18 @@
       <c r="E19" s="110"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="113" t="s">
+      <c r="B20" s="114" t="s">
         <v>381</v>
       </c>
-      <c r="C20" s="113"/>
-      <c r="D20" s="113"/>
+      <c r="C20" s="114"/>
+      <c r="D20" s="114"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="113" t="s">
+      <c r="B21" s="114" t="s">
         <v>388</v>
       </c>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
+      <c r="C21" s="114"/>
+      <c r="D21" s="114"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
@@ -7178,18 +7178,18 @@
       <c r="D26" s="5"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B28" s="113" t="s">
+      <c r="B28" s="114" t="s">
         <v>394</v>
       </c>
-      <c r="C28" s="113"/>
-      <c r="D28" s="113"/>
+      <c r="C28" s="114"/>
+      <c r="D28" s="114"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="113" t="s">
+      <c r="B29" s="114" t="s">
         <v>389</v>
       </c>
-      <c r="C29" s="113"/>
-      <c r="D29" s="113"/>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
@@ -7225,18 +7225,18 @@
       <c r="D34" s="5"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="115" t="s">
+      <c r="B35" s="116" t="s">
         <v>390</v>
       </c>
-      <c r="C35" s="115"/>
-      <c r="D35" s="115"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="116"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="114" t="s">
+      <c r="B36" s="115" t="s">
         <v>391</v>
       </c>
-      <c r="C36" s="114"/>
-      <c r="D36" s="114"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="115"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="101" t="s">
@@ -7268,20 +7268,20 @@
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="112" t="s">
+      <c r="B41" s="113" t="s">
         <v>399</v>
       </c>
-      <c r="C41" s="112"/>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
+      <c r="C41" s="113"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="113"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="112" t="s">
+      <c r="B42" s="113" t="s">
         <v>403</v>
       </c>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
+      <c r="C42" s="113"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="113"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -7327,12 +7327,12 @@
     <mergeCell ref="B3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="20" priority="2">
       <formula>$Q44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="19" priority="1">
       <formula>$Q44=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7343,10 +7343,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A3CB9E-ED1A-40D2-8190-0A166B48A835}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7354,94 +7354,196 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="79">
         <v>44361</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C1" s="52">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14">
         <v>44362</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C2" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
         <v>44363</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C3" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
         <v>44364</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" s="52">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C4" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>44365</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C5" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>44368</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B6" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C6" s="52">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>44369</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="52">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C7" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>44370</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B8" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C8" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>44371</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B9" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C9" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
         <v>44372</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B10" s="52">
+        <v>0.625</v>
+      </c>
+      <c r="C10" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
         <v>44375</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B11" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C11" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
         <v>44376</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B12" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C12" s="52">
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
         <v>44377</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B13" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C13" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
         <v>44378</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B14" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
         <v>44379</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C15" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
         <v>44382</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C16" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
         <v>44383</v>
       </c>
+      <c r="B17" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C17" s="52">
+        <v>0.875</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7637,7 +7739,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Constrictions can now be marked as hard or weak from the excel. The output file provides data about the exams involved in the constriction.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006BA216-9943-496B-88CE-E9FD57095D1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F399949-7585-4CCF-B4C9-D4C8FDE182D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="26430" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="409">
   <si>
     <t>ID</t>
   </si>
@@ -1318,9 +1318,6 @@
     <t>Interval ending date</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>El examen debe ser fechado en el intervalo de fechas dado</t>
   </si>
   <si>
@@ -1331,6 +1328,15 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>Hard?</t>
+  </si>
+  <si>
+    <t>Exam_id_1_data</t>
+  </si>
+  <si>
+    <t>Exam_id_2_data</t>
   </si>
 </sst>
 </file>
@@ -1915,7 +1921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2063,69 +2069,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -2195,6 +2155,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2221,23 +2232,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2542,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2648,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="92" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="S5" s="112" t="s">
         <v>298</v>
@@ -2706,7 +2717,7 @@
         <v>0</v>
       </c>
       <c r="R6" s="77" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="S6" s="76" t="s">
         <v>253</v>
@@ -2774,9 +2785,7 @@
       <c r="Q7" s="13">
         <v>1</v>
       </c>
-      <c r="R7" s="13" t="s">
-        <v>405</v>
-      </c>
+      <c r="R7" s="13"/>
       <c r="S7" s="12" t="s">
         <v>256</v>
       </c>
@@ -2915,7 +2924,7 @@
         <v>3</v>
       </c>
       <c r="R9" s="13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="S9" s="12" t="s">
         <v>254</v>
@@ -3055,7 +3064,7 @@
         <v>5</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S11" s="12" t="s">
         <v>254</v>
@@ -3191,7 +3200,7 @@
         <v>7</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S13" s="12" t="s">
         <v>255</v>
@@ -3264,7 +3273,7 @@
         <v>8</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="S14" s="12" t="s">
         <v>256</v>
@@ -6931,32 +6940,32 @@
     <mergeCell ref="S5:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="S10 S8:T9 S11:T33 S34 S35:T67 A7:N43 A6:J6 L6:T6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:R67 Q7:T7 O7:P67">
-    <cfRule type="expression" dxfId="26" priority="18">
+    <cfRule type="expression" dxfId="8" priority="18">
       <formula>$U6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S67">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="23" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$S6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>$S44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$S58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6968,10 +6977,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="B2:E44"/>
+  <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6979,25 +6988,29 @@
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="7" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="114" t="s">
         <v>379</v>
       </c>
       <c r="C2" s="114"/>
       <c r="D2" s="114"/>
       <c r="E2" s="114"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="114"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="114" t="s">
         <v>387</v>
       </c>
       <c r="C3" s="114"/>
       <c r="D3" s="114"/>
       <c r="E3" s="114"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="114"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="101" t="s">
         <v>382</v>
       </c>
@@ -7007,11 +7020,20 @@
       <c r="D4" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="E4" s="102" t="s">
+      <c r="E4" s="101" t="s">
+        <v>406</v>
+      </c>
+      <c r="F4" s="102" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G4" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="H4" s="127" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="97">
         <v>0</v>
       </c>
@@ -7021,9 +7043,13 @@
       <c r="D5" s="97">
         <v>1</v>
       </c>
-      <c r="E5" s="40"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="40" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="40"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="98">
         <v>5</v>
       </c>
@@ -7033,9 +7059,13 @@
       <c r="D6" s="98">
         <v>2</v>
       </c>
-      <c r="E6" s="40"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="40" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="40"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="98">
         <v>47</v>
       </c>
@@ -7045,9 +7075,13 @@
       <c r="D7" s="98">
         <v>1</v>
       </c>
-      <c r="E7" s="100"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="40" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="100"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="98">
         <v>0</v>
       </c>
@@ -7057,233 +7091,314 @@
       <c r="D8" s="98">
         <v>5</v>
       </c>
-      <c r="E8" s="100"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="40" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="100"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="103"/>
       <c r="C9" s="71"/>
       <c r="D9" s="103"/>
       <c r="E9" s="85"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="85"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="120" t="s">
         <v>380</v>
       </c>
       <c r="C11" s="121"/>
       <c r="D11" s="122"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="123"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="117" t="s">
         <v>395</v>
       </c>
       <c r="C12" s="118"/>
       <c r="D12" s="119"/>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="123"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
         <v>382</v>
       </c>
       <c r="C13" s="109" t="s">
         <v>383</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" t="s">
+        <v>406</v>
+      </c>
+      <c r="E13" s="107" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="G13" s="127" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="39">
         <v>46</v>
       </c>
       <c r="C14" s="97">
         <v>47</v>
       </c>
-      <c r="D14" s="40"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="40" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="40"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="39">
         <v>34</v>
       </c>
       <c r="C15" s="98">
         <v>23</v>
       </c>
-      <c r="D15" s="40"/>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="40"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="39">
         <v>47</v>
       </c>
       <c r="C16" s="98">
         <v>3</v>
       </c>
-      <c r="D16" s="100"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="100"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="94"/>
       <c r="C17" s="103"/>
-      <c r="D17" s="85"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="110"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="85"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F19" s="110"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="114" t="s">
         <v>381</v>
       </c>
       <c r="C20" s="114"/>
       <c r="D20" s="114"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="123"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="114" t="s">
         <v>388</v>
       </c>
       <c r="C21" s="114"/>
       <c r="D21" s="114"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="123"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
         <v>385</v>
       </c>
       <c r="C22" s="104" t="s">
         <v>386</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" t="s">
+        <v>406</v>
+      </c>
+      <c r="E22" s="102" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="G22" s="127"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="97">
         <v>1</v>
       </c>
       <c r="C23" s="95">
         <v>44364</v>
       </c>
-      <c r="D23" s="97"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="97"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="98">
         <v>2</v>
       </c>
       <c r="C24" s="95">
         <v>44364</v>
       </c>
-      <c r="D24" s="98"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="98"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="105"/>
       <c r="C25" s="96"/>
-      <c r="D25" s="106"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="106"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C26" s="30"/>
       <c r="D26" s="5"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="5"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="114" t="s">
         <v>394</v>
       </c>
       <c r="C28" s="114"/>
       <c r="D28" s="114"/>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="123"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="114" t="s">
         <v>389</v>
       </c>
       <c r="C29" s="114"/>
       <c r="D29" s="114"/>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="123"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
         <v>382</v>
       </c>
       <c r="C30" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="D30" s="102" t="s">
+      <c r="D30" t="s">
+        <v>406</v>
+      </c>
+      <c r="E30" s="102" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="G30" s="127" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="97">
         <v>23</v>
       </c>
       <c r="C31" s="40">
         <v>24</v>
       </c>
-      <c r="D31" s="40"/>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E31" s="40"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="103"/>
       <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="85"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="99"/>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="99"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="116" t="s">
         <v>390</v>
       </c>
       <c r="C35" s="116"/>
       <c r="D35" s="116"/>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="124"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="115" t="s">
         <v>391</v>
       </c>
       <c r="C36" s="115"/>
       <c r="D36" s="115"/>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="125"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="101" t="s">
         <v>392</v>
       </c>
       <c r="C37" s="101" t="s">
         <v>393</v>
       </c>
-      <c r="D37" s="102" t="s">
+      <c r="D37" t="s">
+        <v>406</v>
+      </c>
+      <c r="E37" s="102" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="127" t="s">
+        <v>407</v>
+      </c>
+      <c r="G37" s="127" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="97">
         <v>23</v>
       </c>
       <c r="C38" s="40">
         <v>26</v>
       </c>
-      <c r="D38" s="98"/>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="98"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="103"/>
       <c r="C39" s="85"/>
-      <c r="D39" s="103"/>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="103"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D40" s="99"/>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="99"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="113" t="s">
         <v>399</v>
       </c>
       <c r="C41" s="113"/>
       <c r="D41" s="113"/>
       <c r="E41" s="113"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="113"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="113" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C42" s="113"/>
       <c r="D42" s="113"/>
       <c r="E42" s="113"/>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="113"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>385</v>
       </c>
@@ -7294,10 +7409,17 @@
         <v>401</v>
       </c>
       <c r="E43" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="F43" s="36" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="G43" s="128" t="s">
+        <v>407</v>
+      </c>
+      <c r="H43" s="36"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44">
         <v>53</v>
       </c>
@@ -7307,15 +7429,17 @@
       <c r="D44" s="14">
         <v>44364</v>
       </c>
-      <c r="E44" t="s">
-        <v>402</v>
-      </c>
+      <c r="E44" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="126"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B2:F2"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B29:D29"/>
@@ -7324,16 +7448,11 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="expression" dxfId="20" priority="2">
-      <formula>$Q44=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="19" priority="1">
-      <formula>$Q44=0</formula>
+  <conditionalFormatting sqref="C44:D44 F44">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$R44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7345,8 +7464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A3CB9E-ED1A-40D2-8190-0A166B48A835}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7543,7 +7662,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7739,7 +7858,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Test instance generator adapted to input changes and generates hard constrictions.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F399949-7585-4CCF-B4C9-D4C8FDE182D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38FCD92-7239-4FAA-BF75-D41FAFC2787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -2036,6 +2036,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2069,23 +2081,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2155,57 +2206,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2232,23 +2232,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="17"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="16"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2661,10 +2661,10 @@
       <c r="R5" s="92" t="s">
         <v>403</v>
       </c>
-      <c r="S5" s="112" t="s">
+      <c r="S5" s="118" t="s">
         <v>298</v>
       </c>
-      <c r="T5" s="112"/>
+      <c r="T5" s="118"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -6940,32 +6940,32 @@
     <mergeCell ref="S5:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="S10 S8:T9 S11:T33 S34 S35:T67 A7:N43 A6:J6 L6:T6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:R67 Q7:T7 O7:P67">
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="25" priority="18">
       <formula>$U6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S67">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="22" priority="3">
       <formula>$S6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>$S44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="20" priority="1">
       <formula>$S58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6979,8 +6979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
   <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6993,22 +6993,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="120" t="s">
         <v>379</v>
       </c>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="114"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="114" t="s">
+      <c r="B3" s="120" t="s">
         <v>387</v>
       </c>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="101" t="s">
@@ -7026,10 +7026,10 @@
       <c r="F4" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="G4" s="127" t="s">
+      <c r="G4" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="H4" s="127" t="s">
+      <c r="H4" s="116" t="s">
         <v>408</v>
       </c>
     </row>
@@ -7105,20 +7105,20 @@
       <c r="F9" s="85"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="126" t="s">
         <v>380</v>
       </c>
-      <c r="C11" s="121"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
+      <c r="C11" s="127"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="112"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="123" t="s">
         <v>395</v>
       </c>
-      <c r="C12" s="118"/>
-      <c r="D12" s="119"/>
-      <c r="E12" s="123"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="112"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="108" t="s">
@@ -7133,10 +7133,10 @@
       <c r="E13" s="107" t="s">
         <v>398</v>
       </c>
-      <c r="F13" s="127" t="s">
+      <c r="F13" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="G13" s="127" t="s">
+      <c r="G13" s="116" t="s">
         <v>408</v>
       </c>
     </row>
@@ -7188,20 +7188,20 @@
       <c r="F19" s="110"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="114" t="s">
+      <c r="B20" s="120" t="s">
         <v>381</v>
       </c>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="123"/>
+      <c r="C20" s="120"/>
+      <c r="D20" s="120"/>
+      <c r="E20" s="112"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="114" t="s">
+      <c r="B21" s="120" t="s">
         <v>388</v>
       </c>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="123"/>
+      <c r="C21" s="120"/>
+      <c r="D21" s="120"/>
+      <c r="E21" s="112"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="104" t="s">
@@ -7216,10 +7216,10 @@
       <c r="E22" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="F22" s="127" t="s">
+      <c r="F22" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="G22" s="127"/>
+      <c r="G22" s="116"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="97">
@@ -7258,20 +7258,20 @@
       <c r="E26" s="5"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="114" t="s">
+      <c r="B28" s="120" t="s">
         <v>394</v>
       </c>
-      <c r="C28" s="114"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="123"/>
+      <c r="C28" s="120"/>
+      <c r="D28" s="120"/>
+      <c r="E28" s="112"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="114" t="s">
+      <c r="B29" s="120" t="s">
         <v>389</v>
       </c>
-      <c r="C29" s="114"/>
-      <c r="D29" s="114"/>
-      <c r="E29" s="123"/>
+      <c r="C29" s="120"/>
+      <c r="D29" s="120"/>
+      <c r="E29" s="112"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="101" t="s">
@@ -7286,10 +7286,10 @@
       <c r="E30" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="F30" s="127" t="s">
+      <c r="F30" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="G30" s="127" t="s">
+      <c r="G30" s="116" t="s">
         <v>408</v>
       </c>
     </row>
@@ -7322,20 +7322,20 @@
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="116" t="s">
+      <c r="B35" s="122" t="s">
         <v>390</v>
       </c>
-      <c r="C35" s="116"/>
-      <c r="D35" s="116"/>
-      <c r="E35" s="124"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122"/>
+      <c r="E35" s="113"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="C36" s="115"/>
-      <c r="D36" s="115"/>
-      <c r="E36" s="125"/>
+      <c r="C36" s="121"/>
+      <c r="D36" s="121"/>
+      <c r="E36" s="114"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="101" t="s">
@@ -7350,10 +7350,10 @@
       <c r="E37" s="102" t="s">
         <v>397</v>
       </c>
-      <c r="F37" s="127" t="s">
+      <c r="F37" s="116" t="s">
         <v>407</v>
       </c>
-      <c r="G37" s="127" t="s">
+      <c r="G37" s="116" t="s">
         <v>408</v>
       </c>
     </row>
@@ -7381,22 +7381,22 @@
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="113" t="s">
+      <c r="B41" s="119" t="s">
         <v>399</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="113"/>
-      <c r="E41" s="113"/>
-      <c r="F41" s="113"/>
+      <c r="C41" s="119"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
+      <c r="F41" s="119"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="113" t="s">
+      <c r="B42" s="119" t="s">
         <v>402</v>
       </c>
-      <c r="C42" s="113"/>
-      <c r="D42" s="113"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="113"/>
+      <c r="C42" s="119"/>
+      <c r="D42" s="119"/>
+      <c r="E42" s="119"/>
+      <c r="F42" s="119"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
@@ -7414,7 +7414,7 @@
       <c r="F43" s="36" t="s">
         <v>398</v>
       </c>
-      <c r="G43" s="128" t="s">
+      <c r="G43" s="117" t="s">
         <v>407</v>
       </c>
       <c r="H43" s="36"/>
@@ -7430,10 +7430,10 @@
         <v>44364</v>
       </c>
       <c r="E44" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="F44" s="126"/>
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F44" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -7451,7 +7451,7 @@
     <mergeCell ref="B3:F3"/>
   </mergeCells>
   <conditionalFormatting sqref="C44:D44 F44">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>$R44=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7662,7 +7662,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7858,7 +7858,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Improved error notification to the user.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38FCD92-7239-4FAA-BF75-D41FAFC2787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B9AA00-C1D7-43F0-A14B-C71DA0777CDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -2553,8 +2553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z67"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5435,9 +5435,7 @@
       <c r="Z45" s="40"/>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A46" s="83">
-        <v>1</v>
-      </c>
+      <c r="A46" s="83"/>
       <c r="B46" s="12">
         <v>1</v>
       </c>
@@ -6979,8 +6977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
   <dimension ref="B2:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7050,9 +7048,7 @@
       <c r="F5" s="40"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="98">
-        <v>5</v>
-      </c>
+      <c r="B6" s="98"/>
       <c r="C6" s="5">
         <v>45</v>
       </c>
@@ -7069,9 +7065,7 @@
       <c r="B7" s="98">
         <v>47</v>
       </c>
-      <c r="C7" s="5">
-        <v>2</v>
-      </c>
+      <c r="C7" s="5"/>
       <c r="D7" s="98">
         <v>1</v>
       </c>
@@ -7088,9 +7082,7 @@
       <c r="C8" s="36">
         <v>50</v>
       </c>
-      <c r="D8" s="98">
-        <v>5</v>
-      </c>
+      <c r="D8" s="98"/>
       <c r="E8" s="40" t="b">
         <f>FALSE</f>
         <v>0</v>
@@ -7228,10 +7220,6 @@
       <c r="C23" s="95">
         <v>44364</v>
       </c>
-      <c r="D23" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
       <c r="E23" s="97"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -7423,9 +7411,7 @@
       <c r="B44">
         <v>53</v>
       </c>
-      <c r="C44" s="14">
-        <v>44363</v>
-      </c>
+      <c r="C44" s="14"/>
       <c r="D44" s="14">
         <v>44364</v>
       </c>

</xml_diff>

<commit_message>
Bug error fixes due to TC10 (with file p3.xlsx)
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C09618B-417A-483D-8027-B2BC65640E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297FCC88-EE41-4451-B096-D7EB27EFA0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="420" windowWidth="26430" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1215" yWindow="420" windowWidth="27285" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="409">
   <si>
     <t>ID</t>
   </si>
@@ -1334,6 +1334,9 @@
   </si>
   <si>
     <t>Exam_id_2_data</t>
+  </si>
+  <si>
+    <t>asda</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +1921,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -2013,7 +2016,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
@@ -2045,6 +2047,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2082,57 +2088,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="27">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2203,6 +2165,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2229,23 +2242,23 @@
     <sortCondition ref="F2:F34"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="11"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="1"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Hora de inicio" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hora de finalización" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Correo electrónico" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Nombre" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Asignatura" dataDxfId="21"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Columna1" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo de examen" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Especifique las características de presencialidad" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Nº conv" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Dur." dataDxfId="16"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2º ex" dataDxfId="15"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Tipo del 2º examen" dataDxfId="14"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Especifique las características de presencialidad del 2º examen" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Número máximo estimado de alumnos convocados al 2º examen" dataDxfId="12"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Duración máxima estimada del 2º examen" dataDxfId="11"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Observaciones" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2548,10 +2561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z67"/>
+  <dimension ref="A1:Z72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2709,10 +2722,10 @@
       <c r="R5" s="92" t="s">
         <v>402</v>
       </c>
-      <c r="S5" s="118" t="s">
+      <c r="S5" s="119" t="s">
         <v>297</v>
       </c>
-      <c r="T5" s="118"/>
+      <c r="T5" s="119"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="75">
@@ -3824,7 +3837,7 @@
       <c r="Q22" s="77">
         <v>16</v>
       </c>
-      <c r="R22" s="111"/>
+      <c r="R22" s="110"/>
       <c r="S22" s="65" t="s">
         <v>252</v>
       </c>
@@ -6485,7 +6498,7 @@
       <c r="Q62" s="77">
         <v>56</v>
       </c>
-      <c r="R62" s="111"/>
+      <c r="R62" s="110"/>
       <c r="S62" s="25" t="s">
         <v>296</v>
       </c>
@@ -6733,9 +6746,7 @@
       <c r="P66" s="77">
         <v>0</v>
       </c>
-      <c r="Q66" s="77">
-        <v>60</v>
-      </c>
+      <c r="Q66" s="77"/>
       <c r="R66" s="8"/>
       <c r="S66" s="12" t="s">
         <v>254</v>
@@ -6827,6 +6838,9 @@
       <c r="Y67" s="91" t="s">
         <v>377</v>
       </c>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q72" s="117"/>
     </row>
   </sheetData>
   <autoFilter ref="A5:T67" xr:uid="{00000000-0009-0000-0000-000000000000}">
@@ -6846,32 +6860,32 @@
     <mergeCell ref="S5:T5"/>
   </mergeCells>
   <conditionalFormatting sqref="S10 S8:T9 S11:T33 S34 S35:T67 A7:N43 A6:J6 L6:T6 A45:N57 A44:J44 L44:N44 A59:N67 A58:J58 L58:N58 Q8:R67 Q7:T7 O7:P67">
-    <cfRule type="expression" dxfId="25" priority="18">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>$U6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H67">
-    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Presencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S6:S67">
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"polideportivo"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>$S6=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$S44=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="expression" dxfId="20" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>$S58=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6883,10 +6897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
-  <dimension ref="B2:H44"/>
+  <dimension ref="B2:H43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6899,54 +6913,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="120" t="s">
+      <c r="B2" s="121" t="s">
         <v>378</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="120" t="s">
-        <v>386</v>
-      </c>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
+      <c r="B3" s="118" t="s">
+        <v>408</v>
+      </c>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="101" t="s">
+      <c r="B4" s="100" t="s">
         <v>381</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="100" t="s">
         <v>382</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="100" t="s">
         <v>383</v>
       </c>
-      <c r="E4" s="101" t="s">
+      <c r="E4" s="100" t="s">
         <v>405</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="G4" s="116" t="s">
+      <c r="G4" s="115" t="s">
         <v>406</v>
       </c>
-      <c r="H4" s="116" t="s">
+      <c r="H4" s="115" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="97">
+      <c r="B5" s="96">
         <v>0</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="97">
+      <c r="D5" s="96">
         <v>1</v>
       </c>
       <c r="E5" s="40" t="b">
@@ -6956,11 +6970,13 @@
       <c r="F5" s="40"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="98"/>
+      <c r="B6" s="97">
+        <v>25323</v>
+      </c>
       <c r="C6" s="5">
         <v>45</v>
       </c>
-      <c r="D6" s="98">
+      <c r="D6" s="97">
         <v>2</v>
       </c>
       <c r="E6" s="40" t="b">
@@ -6970,73 +6986,75 @@
       <c r="F6" s="40"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="98">
+      <c r="B7" s="97">
         <v>47</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="98">
+      <c r="C7" s="5">
+        <v>14</v>
+      </c>
+      <c r="D7" s="97">
         <v>1</v>
       </c>
       <c r="E7" s="40" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F7" s="100"/>
+      <c r="F7" s="99"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="98">
+      <c r="B8" s="97">
         <v>0</v>
       </c>
       <c r="C8" s="36">
         <v>50</v>
       </c>
-      <c r="D8" s="98"/>
+      <c r="D8" s="97"/>
       <c r="E8" s="40" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="F8" s="100"/>
+      <c r="F8" s="99"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="103"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="71"/>
-      <c r="D9" s="103"/>
+      <c r="D9" s="102"/>
       <c r="E9" s="85"/>
       <c r="F9" s="85"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="126" t="s">
+      <c r="B11" s="127" t="s">
         <v>379</v>
       </c>
-      <c r="C11" s="127"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="112"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="129"/>
+      <c r="E11" s="111"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="124" t="s">
         <v>394</v>
       </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="112"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="126"/>
+      <c r="E12" s="111"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="107" t="s">
         <v>381</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="108" t="s">
         <v>382</v>
       </c>
       <c r="D13" t="s">
         <v>405</v>
       </c>
-      <c r="E13" s="107" t="s">
+      <c r="E13" s="106" t="s">
         <v>397</v>
       </c>
-      <c r="F13" s="116" t="s">
+      <c r="F13" s="115" t="s">
         <v>406</v>
       </c>
-      <c r="G13" s="116" t="s">
+      <c r="G13" s="115" t="s">
         <v>407</v>
       </c>
     </row>
@@ -7044,7 +7062,7 @@
       <c r="B14" s="39">
         <v>46</v>
       </c>
-      <c r="C14" s="97">
+      <c r="C14" s="96">
         <v>47</v>
       </c>
       <c r="D14" s="40" t="b">
@@ -7057,7 +7075,7 @@
       <c r="B15" s="39">
         <v>34</v>
       </c>
-      <c r="C15" s="98">
+      <c r="C15" s="97">
         <v>23</v>
       </c>
       <c r="D15" t="b">
@@ -7070,283 +7088,287 @@
       <c r="B16" s="39">
         <v>47</v>
       </c>
-      <c r="C16" s="98">
+      <c r="C16" s="97">
         <v>3</v>
       </c>
       <c r="D16" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="E16" s="100"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="94"/>
-      <c r="C17" s="103"/>
-      <c r="E17" s="85"/>
+      <c r="E16" s="99"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F18" s="109"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="110"/>
+      <c r="B19" s="121" t="s">
+        <v>380</v>
+      </c>
+      <c r="C19" s="121"/>
+      <c r="D19" s="121"/>
+      <c r="E19" s="111"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="120" t="s">
-        <v>380</v>
-      </c>
-      <c r="C20" s="120"/>
-      <c r="D20" s="120"/>
-      <c r="E20" s="112"/>
+      <c r="B20" s="121" t="s">
+        <v>387</v>
+      </c>
+      <c r="C20" s="121"/>
+      <c r="D20" s="121"/>
+      <c r="E20" s="111"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="120" t="s">
-        <v>387</v>
-      </c>
-      <c r="C21" s="120"/>
-      <c r="D21" s="120"/>
-      <c r="E21" s="112"/>
+      <c r="B21" s="103" t="s">
+        <v>384</v>
+      </c>
+      <c r="C21" s="103" t="s">
+        <v>385</v>
+      </c>
+      <c r="D21" t="s">
+        <v>405</v>
+      </c>
+      <c r="E21" s="101" t="s">
+        <v>396</v>
+      </c>
+      <c r="F21" s="115" t="s">
+        <v>406</v>
+      </c>
+      <c r="G21" s="115"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="104" t="s">
-        <v>384</v>
-      </c>
-      <c r="C22" s="104" t="s">
-        <v>385</v>
-      </c>
-      <c r="D22" t="s">
-        <v>405</v>
-      </c>
-      <c r="E22" s="102" t="s">
-        <v>396</v>
-      </c>
-      <c r="F22" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="G22" s="116"/>
+      <c r="B22" s="96">
+        <v>1</v>
+      </c>
+      <c r="C22" s="94">
+        <v>44364</v>
+      </c>
+      <c r="D22" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="96"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="97">
-        <v>1</v>
-      </c>
-      <c r="C23" s="95">
+        <v>2</v>
+      </c>
+      <c r="C23" s="94">
         <v>44364</v>
       </c>
+      <c r="D23" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
       <c r="E23" s="97"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="98">
-        <v>2</v>
-      </c>
-      <c r="C24" s="95">
-        <v>44364</v>
-      </c>
-      <c r="D24" t="b">
+      <c r="B24" s="104"/>
+      <c r="C24" s="95"/>
+      <c r="E24" s="105"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="30"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="121" t="s">
+        <v>393</v>
+      </c>
+      <c r="C27" s="121"/>
+      <c r="D27" s="121"/>
+      <c r="E27" s="111"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="121" t="s">
+        <v>388</v>
+      </c>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="111"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="100" t="s">
+        <v>381</v>
+      </c>
+      <c r="C29" s="100" t="s">
+        <v>382</v>
+      </c>
+      <c r="D29" t="s">
+        <v>405</v>
+      </c>
+      <c r="E29" s="101" t="s">
+        <v>396</v>
+      </c>
+      <c r="F29" s="115" t="s">
+        <v>406</v>
+      </c>
+      <c r="G29" s="115" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="96">
+        <v>23</v>
+      </c>
+      <c r="C30" s="40">
+        <v>24</v>
+      </c>
+      <c r="D30" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="E24" s="98"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="105"/>
-      <c r="C25" s="96"/>
-      <c r="E25" s="106"/>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="30"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="120" t="s">
-        <v>393</v>
-      </c>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="112"/>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="120" t="s">
-        <v>388</v>
-      </c>
-      <c r="C29" s="120"/>
-      <c r="D29" s="120"/>
-      <c r="E29" s="112"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="101" t="s">
-        <v>381</v>
-      </c>
-      <c r="C30" s="101" t="s">
-        <v>382</v>
-      </c>
-      <c r="D30" t="s">
-        <v>405</v>
-      </c>
-      <c r="E30" s="102" t="s">
-        <v>396</v>
-      </c>
-      <c r="F30" s="116" t="s">
-        <v>406</v>
-      </c>
-      <c r="G30" s="116" t="s">
-        <v>407</v>
-      </c>
+      <c r="E30" s="40"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B31" s="97">
-        <v>23</v>
-      </c>
-      <c r="C31" s="40">
-        <v>24</v>
-      </c>
-      <c r="D31" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="E31" s="40"/>
+      <c r="B31" s="102"/>
+      <c r="C31" s="85"/>
+      <c r="E31" s="85"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B32" s="103"/>
-      <c r="C32" s="85"/>
-      <c r="E32" s="85"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="99"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="B34" s="123" t="s">
+        <v>389</v>
+      </c>
+      <c r="C34" s="123"/>
+      <c r="D34" s="123"/>
+      <c r="E34" s="112"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="122" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C35" s="122"/>
       <c r="D35" s="122"/>
       <c r="E35" s="113"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="121" t="s">
-        <v>390</v>
-      </c>
-      <c r="C36" s="121"/>
-      <c r="D36" s="121"/>
-      <c r="E36" s="114"/>
+      <c r="B36" s="100" t="s">
+        <v>391</v>
+      </c>
+      <c r="C36" s="100" t="s">
+        <v>392</v>
+      </c>
+      <c r="D36" t="s">
+        <v>405</v>
+      </c>
+      <c r="E36" s="101" t="s">
+        <v>396</v>
+      </c>
+      <c r="F36" s="115" t="s">
+        <v>406</v>
+      </c>
+      <c r="G36" s="115" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="101" t="s">
-        <v>391</v>
-      </c>
-      <c r="C37" s="101" t="s">
-        <v>392</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="B37" s="96">
+        <v>23</v>
+      </c>
+      <c r="C37" s="40">
+        <v>26</v>
+      </c>
+      <c r="D37" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="E37" s="97"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="102"/>
+      <c r="C38" s="85"/>
+      <c r="E38" s="102"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D39" s="98"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="120" t="s">
+        <v>398</v>
+      </c>
+      <c r="C40" s="120"/>
+      <c r="D40" s="120"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="120"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="120" t="s">
+        <v>401</v>
+      </c>
+      <c r="C41" s="120"/>
+      <c r="D41" s="120"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="120"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>384</v>
+      </c>
+      <c r="C42" t="s">
+        <v>399</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E42" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="E37" s="102" t="s">
-        <v>396</v>
-      </c>
-      <c r="F37" s="116" t="s">
+      <c r="F42" s="36" t="s">
+        <v>397</v>
+      </c>
+      <c r="G42" s="116" t="s">
         <v>406</v>
       </c>
-      <c r="G37" s="116" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B38" s="97">
-        <v>23</v>
-      </c>
-      <c r="C38" s="40">
-        <v>26</v>
-      </c>
-      <c r="D38" t="b">
-        <f>FALSE</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="98"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="103"/>
-      <c r="C39" s="85"/>
-      <c r="E39" s="103"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B41" s="119" t="s">
-        <v>398</v>
-      </c>
-      <c r="C41" s="119"/>
-      <c r="D41" s="119"/>
-      <c r="E41" s="119"/>
-      <c r="F41" s="119"/>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="119" t="s">
-        <v>401</v>
-      </c>
-      <c r="C42" s="119"/>
-      <c r="D42" s="119"/>
-      <c r="E42" s="119"/>
-      <c r="F42" s="119"/>
+      <c r="H42" s="36"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
-        <v>384</v>
-      </c>
-      <c r="C43" t="s">
-        <v>399</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="E43" s="36" t="s">
-        <v>405</v>
-      </c>
-      <c r="F43" s="36" t="s">
-        <v>397</v>
-      </c>
-      <c r="G43" s="117" t="s">
-        <v>406</v>
-      </c>
-      <c r="H43" s="36"/>
-    </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44">
+      <c r="B43">
         <v>53</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14">
+      <c r="C43" s="14">
+        <v>44362</v>
+      </c>
+      <c r="D43" s="14">
         <v>44364</v>
       </c>
-      <c r="E44" t="b">
+      <c r="E43" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-      <c r="F44" s="115"/>
+      <c r="F43" s="114"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B42:F42"/>
+  <mergeCells count="11">
     <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B40:F40"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B34:D34"/>
     <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B27:D27"/>
     <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B19:D19"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B3:F3"/>
   </mergeCells>
-  <conditionalFormatting sqref="C44:D44 F44">
-    <cfRule type="expression" dxfId="19" priority="2">
-      <formula>$R44=0</formula>
+  <conditionalFormatting sqref="D43 F43">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$R43=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$Q43=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7358,8 +7380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A3CB9E-ED1A-40D2-8190-0A166B48A835}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7556,7 +7578,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A17">
-    <cfRule type="expression" dxfId="18" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7751,48 +7773,48 @@
       </c>
     </row>
     <row r="26" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J26" s="120" t="s">
+      <c r="J26" s="121" t="s">
         <v>378</v>
       </c>
-      <c r="K26" s="120"/>
-      <c r="L26" s="120"/>
-      <c r="M26" s="120"/>
-      <c r="N26" s="120"/>
+      <c r="K26" s="121"/>
+      <c r="L26" s="121"/>
+      <c r="M26" s="121"/>
+      <c r="N26" s="121"/>
     </row>
     <row r="27" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J27" s="120" t="s">
+      <c r="J27" s="121" t="s">
         <v>386</v>
       </c>
-      <c r="K27" s="120"/>
-      <c r="L27" s="120"/>
-      <c r="M27" s="120"/>
-      <c r="N27" s="120"/>
+      <c r="K27" s="121"/>
+      <c r="L27" s="121"/>
+      <c r="M27" s="121"/>
+      <c r="N27" s="121"/>
     </row>
     <row r="28" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J28" s="101" t="s">
+      <c r="J28" s="100" t="s">
         <v>381</v>
       </c>
-      <c r="K28" s="101" t="s">
+      <c r="K28" s="100" t="s">
         <v>382</v>
       </c>
-      <c r="L28" s="101" t="s">
+      <c r="L28" s="100" t="s">
         <v>383</v>
       </c>
-      <c r="M28" s="101" t="s">
+      <c r="M28" s="100" t="s">
         <v>405</v>
       </c>
-      <c r="N28" s="102" t="s">
+      <c r="N28" s="101" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="29" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J29" s="97">
+      <c r="J29" s="96">
         <v>4</v>
       </c>
       <c r="K29" s="5">
         <v>5</v>
       </c>
-      <c r="L29" s="97">
+      <c r="L29" s="96">
         <v>1</v>
       </c>
       <c r="M29" s="40" t="b">
@@ -7802,11 +7824,11 @@
       <c r="N29" s="40"/>
     </row>
     <row r="30" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J30" s="98"/>
+      <c r="J30" s="97"/>
       <c r="K30" s="5">
         <v>45</v>
       </c>
-      <c r="L30" s="98">
+      <c r="L30" s="97">
         <v>2</v>
       </c>
       <c r="M30" s="40" t="b">
@@ -7816,39 +7838,39 @@
       <c r="N30" s="40"/>
     </row>
     <row r="31" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J31" s="98">
+      <c r="J31" s="97">
         <v>47</v>
       </c>
       <c r="K31" s="5">
         <v>2562</v>
       </c>
-      <c r="L31" s="98">
+      <c r="L31" s="97">
         <v>1</v>
       </c>
       <c r="M31" s="40" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="N31" s="100"/>
+      <c r="N31" s="99"/>
     </row>
     <row r="32" spans="10:14" x14ac:dyDescent="0.25">
-      <c r="J32" s="98">
+      <c r="J32" s="97">
         <v>6</v>
       </c>
       <c r="K32" s="36">
         <v>27</v>
       </c>
-      <c r="L32" s="98">
+      <c r="L32" s="97">
         <v>1</v>
       </c>
       <c r="M32" s="40" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="N32" s="100"/>
+      <c r="N32" s="99"/>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
-      <c r="J33" s="116"/>
+      <c r="J33" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -7856,7 +7878,7 @@
     <mergeCell ref="J27:N27"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C16">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$Q1=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Javadoc fixes. Statistics with headers, Calendar with headers.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sF_numericalComplexity.xlsx
+++ b/files/pruebas/v6_sF_numericalComplexity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297FCC88-EE41-4451-B096-D7EB27EFA0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D87949-8690-43B5-B720-2596CE95FA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1215" yWindow="420" windowWidth="27285" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25515" windowHeight="13935" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="412">
   <si>
     <t>ID</t>
   </si>
@@ -1337,6 +1337,15 @@
   </si>
   <si>
     <t>asda</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Interval Start</t>
+  </si>
+  <si>
+    <t>Interval end</t>
   </si>
 </sst>
 </file>
@@ -2567,7 +2576,7 @@
       <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
@@ -6903,7 +6912,7 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="3" max="3" width="24.85546875" customWidth="1"/>
@@ -7378,42 +7387,42 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A3CB9E-ED1A-40D2-8190-0A166B48A835}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="79">
+      <c r="A1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="79">
         <v>44361</v>
-      </c>
-      <c r="B1" s="52">
-        <v>0.375</v>
-      </c>
-      <c r="C1" s="52">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>44362</v>
       </c>
       <c r="B2" s="52">
         <v>0.375</v>
       </c>
       <c r="C2" s="52">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
-        <v>44363</v>
+        <v>44362</v>
       </c>
       <c r="B3" s="52">
         <v>0.375</v>
@@ -7424,10 +7433,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
-        <v>44364</v>
+        <v>44363</v>
       </c>
       <c r="B4" s="52">
-        <v>0.45833333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C4" s="52">
         <v>0.875</v>
@@ -7435,10 +7444,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
-        <v>44365</v>
+        <v>44364</v>
       </c>
       <c r="B5" s="52">
-        <v>0.375</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="C5" s="52">
         <v>0.875</v>
@@ -7446,32 +7455,32 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>44368</v>
+        <v>44365</v>
       </c>
       <c r="B6" s="52">
         <v>0.375</v>
       </c>
       <c r="C6" s="52">
-        <v>0.83333333333333337</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
-        <v>44369</v>
+        <v>44368</v>
       </c>
       <c r="B7" s="52">
-        <v>0.54166666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="C7" s="52">
-        <v>0.875</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
-        <v>44370</v>
+        <v>44369</v>
       </c>
       <c r="B8" s="52">
-        <v>0.375</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="C8" s="52">
         <v>0.875</v>
@@ -7479,7 +7488,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
-        <v>44371</v>
+        <v>44370</v>
       </c>
       <c r="B9" s="52">
         <v>0.375</v>
@@ -7490,10 +7499,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="14">
-        <v>44372</v>
+        <v>44371</v>
       </c>
       <c r="B10" s="52">
-        <v>0.625</v>
+        <v>0.375</v>
       </c>
       <c r="C10" s="52">
         <v>0.875</v>
@@ -7501,10 +7510,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="14">
-        <v>44375</v>
+        <v>44372</v>
       </c>
       <c r="B11" s="52">
-        <v>0.375</v>
+        <v>0.625</v>
       </c>
       <c r="C11" s="52">
         <v>0.875</v>
@@ -7512,29 +7521,29 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="14">
-        <v>44376</v>
+        <v>44375</v>
       </c>
       <c r="B12" s="52">
         <v>0.375</v>
       </c>
       <c r="C12" s="52">
-        <v>0.79166666666666663</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="14">
-        <v>44377</v>
+        <v>44376</v>
       </c>
       <c r="B13" s="52">
         <v>0.375</v>
       </c>
       <c r="C13" s="52">
-        <v>0.875</v>
+        <v>0.79166666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
-        <v>44378</v>
+        <v>44377</v>
       </c>
       <c r="B14" s="52">
         <v>0.375</v>
@@ -7545,7 +7554,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="14">
-        <v>44379</v>
+        <v>44378</v>
       </c>
       <c r="B15" s="52">
         <v>0.375</v>
@@ -7556,7 +7565,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
-        <v>44382</v>
+        <v>44379</v>
       </c>
       <c r="B16" s="52">
         <v>0.375</v>
@@ -7567,7 +7576,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="14">
-        <v>44383</v>
+        <v>44382</v>
       </c>
       <c r="B17" s="52">
         <v>0.375</v>
@@ -7576,10 +7585,21 @@
         <v>0.875</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="14">
+        <v>44383</v>
+      </c>
+      <c r="B18" s="52">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="52">
+        <v>0.875</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A17">
+  <conditionalFormatting sqref="A2:A18">
     <cfRule type="expression" dxfId="1" priority="1">
-      <formula>$Q1=0</formula>
+      <formula>$Q2=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7594,7 +7614,7 @@
       <selection activeCell="J26" sqref="J26:N33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -7894,7 +7914,7 @@
       <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="5" width="20" hidden="1" customWidth="1"/>
@@ -9459,7 +9479,7 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="30">
@@ -9610,7 +9630,7 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -10254,7 +10274,7 @@
       <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>

</xml_diff>